<commit_message>
Updated slides, shedule, notes
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D11B32-28F7-4A45-81DA-236180DD1CC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38942501-09D3-BD41-A8AC-C28BD396BB98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="-2120" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="163">
   <si>
     <t>Date</t>
   </si>
@@ -291,9 +291,6 @@
     <t>#task-8</t>
   </si>
   <si>
-    <t>Scales</t>
-  </si>
-  <si>
     <t>Summarizing data</t>
   </si>
   <si>
@@ -501,18 +498,12 @@
     <t>Displaying tables</t>
   </si>
   <si>
-    <t>#scales</t>
-  </si>
-  <si>
     <t>slides/10-summarizing-data.html</t>
   </si>
   <si>
     <t>slides/11-reading-data.html</t>
   </si>
   <si>
-    <t>slides/09-scales.html</t>
-  </si>
-  <si>
     <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=0a2cd3fe-e02f-4fd7-a15d-aca8015b9350</t>
   </si>
   <si>
@@ -520,6 +511,18 @@
   </si>
   <si>
     <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=8a5e1ab6-7800-4772-8ff9-aca8017de037</t>
+  </si>
+  <si>
+    <t>#facets</t>
+  </si>
+  <si>
+    <t>slides/09-facets.html</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=b9f18ad7-21a3-4c07-a912-acab001bb44f</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=f751632b-e900-4121-80b8-acab01616c37</t>
   </si>
 </sst>
 </file>
@@ -881,7 +884,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1072,7 +1075,7 @@
         <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L5" t="s">
         <v>37</v>
@@ -1132,7 +1135,7 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K7" t="s">
         <v>33</v>
@@ -1171,7 +1174,7 @@
         <v>41</v>
       </c>
       <c r="K8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L8" t="s">
         <v>42</v>
@@ -1213,7 +1216,7 @@
         <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L9" t="s">
         <v>47</v>
@@ -1282,7 +1285,7 @@
         <v>55</v>
       </c>
       <c r="K11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L11" t="s">
         <v>56</v>
@@ -1324,13 +1327,13 @@
         <v>60</v>
       </c>
       <c r="K12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="L12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1366,13 +1369,13 @@
         <v>59</v>
       </c>
       <c r="K13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="L13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1422,17 +1425,23 @@
       <c r="F15" t="s">
         <v>8</v>
       </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
       <c r="H15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I15" t="s">
         <v>77</v>
       </c>
       <c r="J15" t="s">
-        <v>155</v>
+        <v>151</v>
+      </c>
+      <c r="K15" t="s">
+        <v>162</v>
       </c>
       <c r="L15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M15" t="s">
         <v>78</v>
@@ -1450,7 +1459,7 @@
         <v>44223</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -1458,17 +1467,23 @@
       <c r="F16" t="s">
         <v>8</v>
       </c>
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
       <c r="H16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I16" t="s">
         <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>152</v>
+        <v>159</v>
+      </c>
+      <c r="K16" t="s">
+        <v>161</v>
       </c>
       <c r="L16" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="M16" t="s">
         <v>80</v>
@@ -1486,7 +1501,7 @@
         <v>44225</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17">
         <v>11</v>
@@ -1498,16 +1513,16 @@
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K17" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1522,7 +1537,7 @@
         <v>44223</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F18" t="s">
         <v>64</v>
@@ -1570,7 +1585,7 @@
         <v>44228</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E20">
         <v>12</v>
@@ -1594,7 +1609,7 @@
         <v>44230</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E21">
         <v>13</v>
@@ -1618,7 +1633,7 @@
         <v>44237</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1659,9 +1674,6 @@
         <f t="shared" si="0"/>
         <v>44232</v>
       </c>
-      <c r="D24" t="s">
-        <v>89</v>
-      </c>
       <c r="E24">
         <v>14</v>
       </c>
@@ -1678,7 +1690,7 @@
         <v>44235</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E25">
         <v>15</v>
@@ -1696,7 +1708,7 @@
         <v>44237</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26">
         <v>16</v>
@@ -1741,7 +1753,7 @@
         <v>44239</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E28">
         <v>17</v>
@@ -1759,7 +1771,7 @@
         <v>44249</v>
       </c>
       <c r="D29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E29">
         <v>18</v>
@@ -1777,7 +1789,7 @@
         <v>44251</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E30">
         <v>19</v>
@@ -1795,7 +1807,7 @@
         <v>44251</v>
       </c>
       <c r="D31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -1837,7 +1849,7 @@
         <v>44253</v>
       </c>
       <c r="D33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E33">
         <v>20</v>
@@ -1855,7 +1867,7 @@
         <v>44256</v>
       </c>
       <c r="D34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E34">
         <v>21</v>
@@ -1873,7 +1885,7 @@
         <v>44258</v>
       </c>
       <c r="D35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E35">
         <v>22</v>
@@ -1918,7 +1930,7 @@
         <v>44260</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E37">
         <v>23</v>
@@ -1936,7 +1948,7 @@
         <v>44263</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E38">
         <v>24</v>
@@ -1954,7 +1966,7 @@
         <v>44265</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E39">
         <v>25</v>
@@ -1972,7 +1984,7 @@
         <v>44265</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2014,7 +2026,7 @@
         <v>44267</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E42">
         <v>26</v>
@@ -2032,7 +2044,7 @@
         <v>44267</v>
       </c>
       <c r="D43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -2047,7 +2059,7 @@
         <v>44270</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E44">
         <v>27</v>
@@ -2065,7 +2077,7 @@
         <v>44272</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E45">
         <v>28</v>
@@ -2110,7 +2122,7 @@
         <v>44274</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E47">
         <v>29</v>
@@ -2128,7 +2140,7 @@
         <v>44277</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E48">
         <v>30</v>
@@ -2146,7 +2158,7 @@
         <v>44279</v>
       </c>
       <c r="D49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E49">
         <v>31</v>
@@ -2164,7 +2176,7 @@
         <v>44279</v>
       </c>
       <c r="D50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -2206,7 +2218,7 @@
         <v>44281</v>
       </c>
       <c r="D52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E52">
         <v>32</v>
@@ -2224,7 +2236,7 @@
         <v>44284</v>
       </c>
       <c r="D53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E53">
         <v>33</v>
@@ -2242,7 +2254,7 @@
         <v>44286</v>
       </c>
       <c r="D54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E54">
         <v>34</v>
@@ -2314,7 +2326,7 @@
         <v>44293</v>
       </c>
       <c r="D57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -2329,7 +2341,7 @@
         <v>44295</v>
       </c>
       <c r="D58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
@@ -2344,19 +2356,19 @@
         <v>44215</v>
       </c>
       <c r="D59" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K59" t="s">
         <v>33</v>
       </c>
       <c r="M59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
@@ -2374,10 +2386,10 @@
         <v>63</v>
       </c>
       <c r="F60" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J60" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
@@ -2392,13 +2404,13 @@
         <v>44229</v>
       </c>
       <c r="D61" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F61" t="s">
+        <v>118</v>
+      </c>
+      <c r="J61" t="s">
         <v>119</v>
-      </c>
-      <c r="J61" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
@@ -2413,13 +2425,13 @@
         <v>44236</v>
       </c>
       <c r="D62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F62" t="s">
+        <v>118</v>
+      </c>
+      <c r="J62" t="s">
         <v>119</v>
-      </c>
-      <c r="J62" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -2430,17 +2442,17 @@
         <v>2</v>
       </c>
       <c r="C63" s="1">
-        <f t="shared" ref="C63:C94" si="2">DATEVALUE("2021-01-03")+B63+(A63-1)*7</f>
+        <f t="shared" ref="C63:C75" si="2">DATEVALUE("2021-01-03")+B63+(A63-1)*7</f>
         <v>44257</v>
       </c>
       <c r="D63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F63" t="s">
+        <v>118</v>
+      </c>
+      <c r="J63" t="s">
         <v>119</v>
-      </c>
-      <c r="J63" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
@@ -2455,13 +2467,13 @@
         <v>44271</v>
       </c>
       <c r="D64" t="s">
+        <v>117</v>
+      </c>
+      <c r="F64" t="s">
         <v>118</v>
       </c>
-      <c r="F64" t="s">
+      <c r="J64" t="s">
         <v>119</v>
-      </c>
-      <c r="J64" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -2476,13 +2488,13 @@
         <v>44285</v>
       </c>
       <c r="D65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F65" t="s">
+        <v>118</v>
+      </c>
+      <c r="J65" t="s">
         <v>119</v>
-      </c>
-      <c r="J65" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -2497,13 +2509,13 @@
         <v>44207</v>
       </c>
       <c r="D66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F66" t="s">
+        <v>126</v>
+      </c>
+      <c r="J66" t="s">
         <v>127</v>
-      </c>
-      <c r="J66" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -2518,13 +2530,13 @@
         <v>44214</v>
       </c>
       <c r="D67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -2539,10 +2551,10 @@
         <v>44221</v>
       </c>
       <c r="D68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J68" t="s">
         <v>57</v>
@@ -2560,7 +2572,7 @@
         <v>44228</v>
       </c>
       <c r="D69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
@@ -2575,7 +2587,7 @@
         <v>44235</v>
       </c>
       <c r="D70" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -2590,7 +2602,7 @@
         <v>44249</v>
       </c>
       <c r="D71" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -2605,7 +2617,7 @@
         <v>44256</v>
       </c>
       <c r="D72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -2620,7 +2632,7 @@
         <v>44263</v>
       </c>
       <c r="D73" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -2635,7 +2647,7 @@
         <v>44270</v>
       </c>
       <c r="D74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -2650,7 +2662,7 @@
         <v>44277</v>
       </c>
       <c r="D75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized task 5 and 6
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38942501-09D3-BD41-A8AC-C28BD396BB98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C2EE92-A102-AA4B-A86B-46770744363C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="-2120" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="164">
   <si>
     <t>Date</t>
   </si>
@@ -523,6 +523,9 @@
   </si>
   <si>
     <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=f751632b-e900-4121-80b8-acab01616c37</t>
+  </si>
+  <si>
+    <t>https://classroom.github.com/a/lrSAY6Z8</t>
   </si>
 </sst>
 </file>
@@ -881,10 +884,10 @@
   <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E49" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomRight" activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2574,6 +2577,12 @@
       <c r="D69" t="s">
         <v>146</v>
       </c>
+      <c r="F69" t="s">
+        <v>118</v>
+      </c>
+      <c r="J69" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70">

</xml_diff>

<commit_message>
Revised task 4 video and slides link
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EA11AB-01BA-9946-9FA0-14DFE0FE4FF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6098CEE-6D1C-844C-A5B5-5DF6C7A29274}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="-2120" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="170">
   <si>
     <t>Date</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>#help</t>
+  </si>
+  <si>
+    <t>#task-b6</t>
   </si>
 </sst>
 </file>
@@ -902,7 +905,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1719,8 +1722,14 @@
       <c r="F24" t="s">
         <v>8</v>
       </c>
+      <c r="I24" t="s">
+        <v>21</v>
+      </c>
       <c r="J24" t="s">
         <v>168</v>
+      </c>
+      <c r="M24" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revised schedule, vcs video link
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6098CEE-6D1C-844C-A5B5-5DF6C7A29274}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C2B0E7-53CE-384C-B64A-6F3B4C386C77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="-2120" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="166">
   <si>
     <t>Date</t>
   </si>
@@ -390,18 +390,9 @@
     <t>Assignment 5</t>
   </si>
   <si>
-    <t>Get repo</t>
-  </si>
-  <si>
-    <t>TBA</t>
-  </si>
-  <si>
     <t>Task 4 demo</t>
   </si>
   <si>
-    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=540e63cc-65b7-441f-b234-aca60134e6bd</t>
-  </si>
-  <si>
     <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=c505f402-4ffc-421a-8d3f-aca3017cef01</t>
   </si>
   <si>
@@ -423,9 +414,6 @@
     <t>https://dal.brightspace.com/d2l/le/content/159870/viewContent/2124174/View</t>
   </si>
   <si>
-    <t>https://classroom.github.com/a/Qb-MKdW3</t>
-  </si>
-  <si>
     <t>Nothing to submit</t>
   </si>
   <si>
@@ -525,9 +513,6 @@
     <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=f751632b-e900-4121-80b8-acab01616c37</t>
   </si>
   <si>
-    <t>https://classroom.github.com/a/lrSAY6Z8</t>
-  </si>
-  <si>
     <t>#task-b5</t>
   </si>
   <si>
@@ -544,6 +529,9 @@
   </si>
   <si>
     <t>#task-b6</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=7cb26d66-a26e-4b24-89b1-acaf01321690</t>
   </si>
 </sst>
 </file>
@@ -905,7 +893,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1096,7 +1084,7 @@
         <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L5" t="s">
         <v>37</v>
@@ -1195,7 +1183,7 @@
         <v>41</v>
       </c>
       <c r="K8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L8" t="s">
         <v>42</v>
@@ -1237,7 +1225,7 @@
         <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L9" t="s">
         <v>47</v>
@@ -1306,7 +1294,7 @@
         <v>55</v>
       </c>
       <c r="K11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L11" t="s">
         <v>56</v>
@@ -1348,13 +1336,13 @@
         <v>60</v>
       </c>
       <c r="K12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="L12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="M12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1390,13 +1378,13 @@
         <v>59</v>
       </c>
       <c r="K13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="L13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="M13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1456,13 +1444,13 @@
         <v>77</v>
       </c>
       <c r="J15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K15" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="L15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="M15" t="s">
         <v>78</v>
@@ -1498,13 +1486,13 @@
         <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="M16" t="s">
         <v>80</v>
@@ -1540,16 +1528,16 @@
         <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="L17" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="M17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1564,7 +1552,7 @@
         <v>44223</v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F18" t="s">
         <v>64</v>
@@ -1624,7 +1612,7 @@
         <v>81</v>
       </c>
       <c r="J20" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="M20" t="s">
         <v>82</v>
@@ -1642,7 +1630,7 @@
         <v>44230</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E21">
         <v>13</v>
@@ -1654,7 +1642,7 @@
         <v>83</v>
       </c>
       <c r="J21" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="M21" t="s">
         <v>84</v>
@@ -1672,7 +1660,7 @@
         <v>44237</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1714,7 +1702,7 @@
         <v>44232</v>
       </c>
       <c r="D24" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E24">
         <v>14</v>
@@ -1726,10 +1714,10 @@
         <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="M24" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1861,7 +1849,7 @@
         <v>44251</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -2038,7 +2026,7 @@
         <v>44265</v>
       </c>
       <c r="D40" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2230,7 +2218,7 @@
         <v>44279</v>
       </c>
       <c r="D50" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -2380,7 +2368,7 @@
         <v>44293</v>
       </c>
       <c r="D57" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -2416,13 +2404,13 @@
         <v>111</v>
       </c>
       <c r="I59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K59" t="s">
         <v>33</v>
       </c>
       <c r="M59" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
@@ -2438,12 +2426,6 @@
       </c>
       <c r="D60" t="s">
         <v>63</v>
-      </c>
-      <c r="F60" t="s">
-        <v>118</v>
-      </c>
-      <c r="J60" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
@@ -2460,12 +2442,6 @@
       <c r="D61" t="s">
         <v>113</v>
       </c>
-      <c r="F61" t="s">
-        <v>118</v>
-      </c>
-      <c r="J61" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
@@ -2481,12 +2457,6 @@
       <c r="D62" t="s">
         <v>115</v>
       </c>
-      <c r="F62" t="s">
-        <v>118</v>
-      </c>
-      <c r="J62" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
@@ -2502,12 +2472,6 @@
       <c r="D63" t="s">
         <v>116</v>
       </c>
-      <c r="F63" t="s">
-        <v>118</v>
-      </c>
-      <c r="J63" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
@@ -2523,12 +2487,6 @@
       <c r="D64" t="s">
         <v>117</v>
       </c>
-      <c r="F64" t="s">
-        <v>118</v>
-      </c>
-      <c r="J64" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
@@ -2544,12 +2502,6 @@
       <c r="D65" t="s">
         <v>114</v>
       </c>
-      <c r="F65" t="s">
-        <v>118</v>
-      </c>
-      <c r="J65" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
@@ -2563,13 +2515,13 @@
         <v>44207</v>
       </c>
       <c r="D66" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F66" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J66" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -2584,13 +2536,13 @@
         <v>44214</v>
       </c>
       <c r="D67" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F67" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J67" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -2605,10 +2557,10 @@
         <v>44221</v>
       </c>
       <c r="D68" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F68" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J68" t="s">
         <v>57</v>
@@ -2626,13 +2578,7 @@
         <v>44228</v>
       </c>
       <c r="D69" t="s">
-        <v>146</v>
-      </c>
-      <c r="F69" t="s">
-        <v>118</v>
-      </c>
-      <c r="J69" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
@@ -2647,7 +2593,7 @@
         <v>44235</v>
       </c>
       <c r="D70" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -2662,7 +2608,7 @@
         <v>44249</v>
       </c>
       <c r="D71" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -2677,7 +2623,7 @@
         <v>44256</v>
       </c>
       <c r="D72" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -2692,7 +2638,7 @@
         <v>44263</v>
       </c>
       <c r="D73" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -2707,7 +2653,7 @@
         <v>44270</v>
       </c>
       <c r="D74" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -2722,7 +2668,7 @@
         <v>44277</v>
       </c>
       <c r="D75" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
live coding 2 session
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C2B0E7-53CE-384C-B64A-6F3B4C386C77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1676B42-E44E-F045-8DAB-F6006674329B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="-2120" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -225,9 +225,6 @@
     <t>#sync-2</t>
   </si>
   <si>
-    <t>Assignment 1</t>
-  </si>
-  <si>
     <t>Instructions</t>
   </si>
   <si>
@@ -375,21 +372,6 @@
     <t>Office hour: highlight help with task 4</t>
   </si>
   <si>
-    <t>Assignment 2</t>
-  </si>
-  <si>
-    <t>Assignment 6</t>
-  </si>
-  <si>
-    <t>Assignment 3</t>
-  </si>
-  <si>
-    <t>Assignment 4</t>
-  </si>
-  <si>
-    <t>Assignment 5</t>
-  </si>
-  <si>
     <t>Task 4 demo</t>
   </si>
   <si>
@@ -532,6 +514,24 @@
   </si>
   <si>
     <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=7cb26d66-a26e-4b24-89b1-acaf01321690</t>
+  </si>
+  <si>
+    <t>Assignment 2 available</t>
+  </si>
+  <si>
+    <t>Assignment 1 available</t>
+  </si>
+  <si>
+    <t>Assignment 3 available</t>
+  </si>
+  <si>
+    <t>Assignment 4 available</t>
+  </si>
+  <si>
+    <t>Assignment 5 available</t>
+  </si>
+  <si>
+    <t>Assignment 6 available</t>
   </si>
 </sst>
 </file>
@@ -890,10 +890,10 @@
   <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E22" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K59" sqref="K59"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,7 +954,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C30" si="0">DATEVALUE("2021-01-03")+B2+(A2-1)*7</f>
+        <f>DATEVALUE("2021-01-03")+B2+(A2-1)*7</f>
         <v>44202</v>
       </c>
       <c r="D2" t="s">
@@ -990,7 +990,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" si="0"/>
+        <f>DATEVALUE("2021-01-03")+B3+(A3-1)*7</f>
         <v>44203</v>
       </c>
       <c r="D3" t="s">
@@ -1032,7 +1032,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
+        <f>DATEVALUE("2021-01-03")+B4+(A4-1)*7</f>
         <v>44203</v>
       </c>
       <c r="D4" t="s">
@@ -1059,7 +1059,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
+        <f>DATEVALUE("2021-01-03")+B5+(A5-1)*7</f>
         <v>44204</v>
       </c>
       <c r="D5" t="s">
@@ -1084,7 +1084,7 @@
         <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="L5" t="s">
         <v>37</v>
@@ -1101,32 +1101,17 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
+        <f>DATEVALUE("2021-01-03")+B6+(A6-1)*7</f>
         <v>44207</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
+        <v>133</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1134,20 +1119,35 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>44208</v>
+        <f>DATEVALUE("2021-01-03")+B7+(A7-1)*7</f>
+        <v>44207</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>111</v>
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="M7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1155,41 +1155,20 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="0"/>
-        <v>44209</v>
+        <f>DATEVALUE("2021-01-03")+B8+(A8-1)*7</f>
+        <v>44208</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="K8" t="s">
-        <v>121</v>
-      </c>
-      <c r="L8" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1197,17 +1176,17 @@
         <v>2</v>
       </c>
       <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <f>DATEVALUE("2021-01-03")+B9+(A9-1)*7</f>
+        <v>44209</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
         <v>4</v>
-      </c>
-      <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>44210</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -1219,19 +1198,19 @@
         <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="M9" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1242,65 +1221,65 @@
         <v>4</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="0"/>
+        <f>DATEVALUE("2021-01-03")+B10+(A10-1)*7</f>
         <v>44210</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>45</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>21</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>114</v>
+      </c>
+      <c r="L10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="0"/>
-        <v>44214</v>
+        <f>DATEVALUE("2021-01-03")+B11+(A11-1)*7</f>
+        <v>44210</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="J11" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="K11" t="s">
-        <v>119</v>
-      </c>
-      <c r="L11" t="s">
-        <v>56</v>
-      </c>
-      <c r="M11" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1308,41 +1287,20 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="0"/>
-        <v>44215</v>
+        <f>DATEVALUE("2021-01-03")+B12+(A12-1)*7</f>
+        <v>44214</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12">
-        <v>7</v>
+        <v>134</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="J12" t="s">
-        <v>60</v>
-      </c>
-      <c r="K12" t="s">
-        <v>152</v>
-      </c>
-      <c r="L12" t="s">
-        <v>146</v>
-      </c>
-      <c r="M12" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1350,17 +1308,17 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="0"/>
-        <v>44216</v>
+        <f>DATEVALUE("2021-01-03")+B13+(A13-1)*7</f>
+        <v>44214</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -1372,19 +1330,19 @@
         <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="J13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K13" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="L13" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="M13" t="s">
-        <v>144</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1392,128 +1350,101 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="0"/>
-        <v>44217</v>
+        <f>DATEVALUE("2021-01-03")+B14+(A14-1)*7</f>
+        <v>44215</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>58</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" t="s">
+        <v>21</v>
       </c>
       <c r="J14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>33</v>
+        <v>146</v>
+      </c>
+      <c r="L14" t="s">
+        <v>140</v>
+      </c>
+      <c r="M14" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="0"/>
-        <v>44221</v>
+        <f>DATEVALUE("2021-01-03")+B15+(A15-1)*7</f>
+        <v>44215</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15">
-        <v>9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="G15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
       <c r="I15" t="s">
-        <v>77</v>
-      </c>
-      <c r="J15" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="K15" t="s">
-        <v>158</v>
-      </c>
-      <c r="L15" t="s">
-        <v>150</v>
+        <v>33</v>
       </c>
       <c r="M15" t="s">
-        <v>78</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="0"/>
-        <v>44223</v>
+        <f>DATEVALUE("2021-01-03")+B16+(A16-1)*7</f>
+        <v>44214</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" t="s">
-        <v>3</v>
-      </c>
-      <c r="H16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" t="s">
-        <v>79</v>
-      </c>
-      <c r="J16" t="s">
-        <v>155</v>
-      </c>
-      <c r="K16" t="s">
-        <v>157</v>
-      </c>
-      <c r="L16" t="s">
-        <v>156</v>
-      </c>
-      <c r="M16" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="0"/>
-        <v>44225</v>
+        <f>DATEVALUE("2021-01-03")+B17+(A17-1)*7</f>
+        <v>44216</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="E17">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -1528,37 +1459,43 @@
         <v>21</v>
       </c>
       <c r="J17" t="s">
+        <v>59</v>
+      </c>
+      <c r="K17" t="s">
         <v>148</v>
       </c>
-      <c r="K17" t="s">
-        <v>153</v>
-      </c>
       <c r="L17" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="M17" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
         <v>4</v>
       </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
       <c r="C18" s="1">
-        <f t="shared" si="0"/>
-        <v>44223</v>
+        <f>DATEVALUE("2021-01-03")+B18+(A18-1)*7</f>
+        <v>44217</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>52</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -1566,113 +1503,137 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="0"/>
-        <v>44224</v>
+        <f>DATEVALUE("2021-01-03")+B19+(A19-1)*7</f>
+        <v>44221</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>84</v>
+      </c>
+      <c r="E19">
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>76</v>
       </c>
       <c r="J19" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="K19" t="s">
-        <v>33</v>
+        <v>152</v>
+      </c>
+      <c r="L19" t="s">
+        <v>144</v>
+      </c>
+      <c r="M19" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="0"/>
-        <v>44228</v>
+        <f>DATEVALUE("2021-01-03")+B20+(A20-1)*7</f>
+        <v>44221</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20">
-        <v>12</v>
+        <v>135</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="J20" t="s">
-        <v>160</v>
-      </c>
-      <c r="M20" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="0"/>
-        <v>44230</v>
+        <f>DATEVALUE("2021-01-03")+B21+(A21-1)*7</f>
+        <v>44223</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>87</v>
       </c>
       <c r="E21">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
       </c>
+      <c r="G21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J21" t="s">
-        <v>161</v>
+        <v>149</v>
+      </c>
+      <c r="K21" t="s">
+        <v>151</v>
+      </c>
+      <c r="L21" t="s">
+        <v>150</v>
       </c>
       <c r="M21" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="0"/>
-        <v>44237</v>
+        <f>DATEVALUE("2021-01-03")+B22+(A22-1)*7</f>
+        <v>44223</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>121</v>
+      </c>
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="0"/>
-        <v>44231</v>
+        <f>DATEVALUE("2021-01-03")+B23+(A23-1)*7</f>
+        <v>44224</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -1684,7 +1645,7 @@
         <v>52</v>
       </c>
       <c r="J23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K23" t="s">
         <v>33</v>
@@ -1692,257 +1653,284 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24">
         <v>5</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="0"/>
-        <v>44232</v>
+        <f>DATEVALUE("2021-01-03")+B24+(A24-1)*7</f>
+        <v>44225</v>
       </c>
       <c r="D24" t="s">
-        <v>162</v>
+        <v>85</v>
       </c>
       <c r="E24">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
+      <c r="G24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" t="s">
+        <v>19</v>
+      </c>
       <c r="I24" t="s">
         <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>163</v>
+        <v>142</v>
+      </c>
+      <c r="K24" t="s">
+        <v>147</v>
+      </c>
+      <c r="L24" t="s">
+        <v>145</v>
       </c>
       <c r="M24" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="0"/>
-        <v>44235</v>
+        <f>DATEVALUE("2021-01-03")+B25+(A25-1)*7</f>
+        <v>44228</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25">
-        <v>15</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="0"/>
-        <v>44237</v>
+        <f>DATEVALUE("2021-01-03")+B26+(A26-1)*7</f>
+        <v>44228</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E26">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26" t="s">
+        <v>154</v>
+      </c>
+      <c r="M26" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="0"/>
-        <v>44238</v>
+        <f>DATEVALUE("2021-01-03")+B27+(A27-1)*7</f>
+        <v>44229</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" t="s">
-        <v>52</v>
-      </c>
-      <c r="J27" t="s">
-        <v>69</v>
-      </c>
-      <c r="K27" t="s">
-        <v>33</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="0"/>
-        <v>44239</v>
+        <f>DATEVALUE("2021-01-03")+B28+(A28-1)*7</f>
+        <v>44230</v>
       </c>
       <c r="D28" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="E28">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" t="s">
+        <v>82</v>
+      </c>
+      <c r="J28" t="s">
+        <v>155</v>
+      </c>
+      <c r="M28" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="0"/>
-        <v>44249</v>
+        <f>DATEVALUE("2021-01-03")+B29+(A29-1)*7</f>
+        <v>44231</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>52</v>
+      </c>
+      <c r="J29" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1">
+        <f>DATEVALUE("2021-01-03")+B30+(A30-1)*7</f>
+        <v>44231</v>
+      </c>
+      <c r="D30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E30">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
         <v>8</v>
       </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30" s="1">
-        <f t="shared" si="0"/>
-        <v>44251</v>
-      </c>
-      <c r="D30" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30">
-        <v>19</v>
+      <c r="I30" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" t="s">
+        <v>157</v>
+      </c>
+      <c r="M30" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ref="C31:C62" si="1">DATEVALUE("2021-01-03")+B31+(A31-1)*7</f>
-        <v>44251</v>
+        <f>DATEVALUE("2021-01-03")+B31+(A31-1)*7</f>
+        <v>44235</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="1"/>
-        <v>44252</v>
+        <f>DATEVALUE("2021-01-03")+B32+(A32-1)*7</f>
+        <v>44235</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" t="s">
-        <v>52</v>
-      </c>
-      <c r="J32" t="s">
-        <v>70</v>
-      </c>
-      <c r="K32" t="s">
-        <v>33</v>
+        <v>89</v>
+      </c>
+      <c r="E32">
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="1"/>
-        <v>44253</v>
+        <f>DATEVALUE("2021-01-03")+B33+(A33-1)*7</f>
+        <v>44236</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33">
-        <v>20</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="1"/>
-        <v>44256</v>
+        <f>DATEVALUE("2021-01-03")+B34+(A34-1)*7</f>
+        <v>44237</v>
       </c>
       <c r="D34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E34">
-        <v>21</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" si="1"/>
-        <v>44258</v>
+        <f>DATEVALUE("2021-01-03")+B35+(A35-1)*7</f>
+        <v>44237</v>
       </c>
       <c r="D35" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E35">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B36">
         <v>4</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" si="1"/>
-        <v>44259</v>
+        <f>DATEVALUE("2021-01-03")+B36+(A36-1)*7</f>
+        <v>44238</v>
       </c>
       <c r="D36" t="s">
         <v>10</v>
@@ -1954,7 +1942,7 @@
         <v>52</v>
       </c>
       <c r="J36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K36" t="s">
         <v>33</v>
@@ -1962,718 +1950,730 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B37">
         <v>5</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" si="1"/>
-        <v>44260</v>
+        <f>DATEVALUE("2021-01-03")+B37+(A37-1)*7</f>
+        <v>44239</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E37">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" si="1"/>
-        <v>44263</v>
+        <f>DATEVALUE("2021-01-03")+B38+(A38-1)*7</f>
+        <v>44249</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
-      </c>
-      <c r="E38">
-        <v>24</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" si="1"/>
-        <v>44265</v>
+        <f>DATEVALUE("2021-01-03")+B39+(A39-1)*7</f>
+        <v>44249</v>
       </c>
       <c r="D39" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E39">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" si="1"/>
-        <v>44265</v>
+        <f>DATEVALUE("2021-01-03")+B40+(A40-1)*7</f>
+        <v>44251</v>
       </c>
       <c r="D40" t="s">
-        <v>130</v>
+        <v>93</v>
+      </c>
+      <c r="E40">
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" si="1"/>
-        <v>44266</v>
+        <f>DATEVALUE("2021-01-03")+B41+(A41-1)*7</f>
+        <v>44251</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" t="s">
-        <v>52</v>
-      </c>
-      <c r="J41" t="s">
-        <v>72</v>
-      </c>
-      <c r="K41" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1">
+        <f>DATEVALUE("2021-01-03")+B42+(A42-1)*7</f>
+        <v>44252</v>
+      </c>
+      <c r="D42" t="s">
         <v>10</v>
       </c>
-      <c r="B42">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1">
-        <f t="shared" si="1"/>
-        <v>44267</v>
-      </c>
-      <c r="D42" t="s">
-        <v>100</v>
-      </c>
-      <c r="E42">
-        <v>26</v>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>52</v>
+      </c>
+      <c r="J42" t="s">
+        <v>69</v>
+      </c>
+      <c r="K42" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B43">
         <v>5</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" si="1"/>
-        <v>44267</v>
+        <f>DATEVALUE("2021-01-03")+B43+(A43-1)*7</f>
+        <v>44253</v>
       </c>
       <c r="D43" t="s">
-        <v>109</v>
+        <v>94</v>
+      </c>
+      <c r="E43">
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" si="1"/>
-        <v>44270</v>
+        <f>DATEVALUE("2021-01-03")+B44+(A44-1)*7</f>
+        <v>44256</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
-      </c>
-      <c r="E44">
-        <v>27</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" si="1"/>
-        <v>44272</v>
+        <f>DATEVALUE("2021-01-03")+B45+(A45-1)*7</f>
+        <v>44256</v>
       </c>
       <c r="D45" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E45">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" si="1"/>
-        <v>44273</v>
+        <f>DATEVALUE("2021-01-03")+B46+(A46-1)*7</f>
+        <v>44257</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
-      </c>
-      <c r="F46" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" t="s">
-        <v>52</v>
-      </c>
-      <c r="J46" t="s">
-        <v>73</v>
-      </c>
-      <c r="K46" t="s">
-        <v>33</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B47">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" si="1"/>
-        <v>44274</v>
+        <f>DATEVALUE("2021-01-03")+B47+(A47-1)*7</f>
+        <v>44258</v>
       </c>
       <c r="D47" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E47">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" si="1"/>
-        <v>44277</v>
+        <f>DATEVALUE("2021-01-03")+B48+(A48-1)*7</f>
+        <v>44259</v>
       </c>
       <c r="D48" t="s">
-        <v>104</v>
-      </c>
-      <c r="E48">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" t="s">
+        <v>52</v>
+      </c>
+      <c r="J48" t="s">
+        <v>70</v>
+      </c>
+      <c r="K48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" si="1"/>
-        <v>44279</v>
+        <f>DATEVALUE("2021-01-03")+B49+(A49-1)*7</f>
+        <v>44260</v>
       </c>
       <c r="D49" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E49">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" si="1"/>
-        <v>44279</v>
+        <f>DATEVALUE("2021-01-03")+B50+(A50-1)*7</f>
+        <v>44263</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1">
+        <f>DATEVALUE("2021-01-03")+B51+(A51-1)*7</f>
+        <v>44263</v>
+      </c>
+      <c r="D51" t="s">
+        <v>97</v>
+      </c>
+      <c r="E51">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1">
+        <f>DATEVALUE("2021-01-03")+B52+(A52-1)*7</f>
+        <v>44265</v>
+      </c>
+      <c r="D52" t="s">
+        <v>98</v>
+      </c>
+      <c r="E52">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" s="1">
+        <f>DATEVALUE("2021-01-03")+B53+(A53-1)*7</f>
+        <v>44265</v>
+      </c>
+      <c r="D53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54">
         <v>4</v>
       </c>
-      <c r="C51" s="1">
-        <f t="shared" si="1"/>
-        <v>44280</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="C54" s="1">
+        <f>DATEVALUE("2021-01-03")+B54+(A54-1)*7</f>
+        <v>44266</v>
+      </c>
+      <c r="D54" t="s">
         <v>10</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F54" t="s">
         <v>11</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G54" t="s">
         <v>52</v>
       </c>
-      <c r="J51" t="s">
-        <v>74</v>
-      </c>
-      <c r="K51" t="s">
+      <c r="J54" t="s">
+        <v>71</v>
+      </c>
+      <c r="K54" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>12</v>
-      </c>
-      <c r="B52">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>10</v>
+      </c>
+      <c r="B55">
         <v>5</v>
       </c>
-      <c r="C52" s="1">
-        <f t="shared" si="1"/>
-        <v>44281</v>
-      </c>
-      <c r="D52" t="s">
-        <v>106</v>
-      </c>
-      <c r="E52">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>13</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53" s="1">
-        <f t="shared" si="1"/>
-        <v>44284</v>
-      </c>
-      <c r="D53" t="s">
-        <v>107</v>
-      </c>
-      <c r="E53">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>13</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="C54" s="1">
-        <f t="shared" si="1"/>
-        <v>44286</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="C55" s="1">
+        <f>DATEVALUE("2021-01-03")+B55+(A55-1)*7</f>
+        <v>44267</v>
+      </c>
+      <c r="D55" t="s">
+        <v>99</v>
+      </c>
+      <c r="E55">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>10</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56" s="1">
+        <f>DATEVALUE("2021-01-03")+B56+(A56-1)*7</f>
+        <v>44267</v>
+      </c>
+      <c r="D56" t="s">
         <v>108</v>
       </c>
-      <c r="E54">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>13</v>
-      </c>
-      <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="C55" s="1">
-        <f t="shared" si="1"/>
-        <v>44287</v>
-      </c>
-      <c r="D55" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" t="s">
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57">
         <v>11</v>
       </c>
-      <c r="G55" t="s">
-        <v>52</v>
-      </c>
-      <c r="J55" t="s">
-        <v>48</v>
-      </c>
-      <c r="K55" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>14</v>
-      </c>
-      <c r="B56">
-        <v>2</v>
-      </c>
-      <c r="C56" s="1">
-        <f t="shared" si="1"/>
-        <v>44292</v>
-      </c>
-      <c r="D56" t="s">
-        <v>53</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1">
+        <f>DATEVALUE("2021-01-03")+B57+(A57-1)*7</f>
+        <v>44270</v>
+      </c>
+      <c r="D57" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58">
         <v>11</v>
       </c>
-      <c r="G56" t="s">
-        <v>52</v>
-      </c>
-      <c r="J56" t="s">
-        <v>49</v>
-      </c>
-      <c r="K56" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>14</v>
-      </c>
-      <c r="B57">
-        <v>3</v>
-      </c>
-      <c r="C57" s="1">
-        <f t="shared" si="1"/>
-        <v>44293</v>
-      </c>
-      <c r="D57" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>14</v>
-      </c>
       <c r="B58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C58" s="1">
-        <f t="shared" si="1"/>
-        <v>44295</v>
+        <f>DATEVALUE("2021-01-03")+B58+(A58-1)*7</f>
+        <v>44270</v>
       </c>
       <c r="D58" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="E58">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B59">
         <v>2</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" si="1"/>
-        <v>44215</v>
+        <f>DATEVALUE("2021-01-03")+B59+(A59-1)*7</f>
+        <v>44271</v>
       </c>
       <c r="D59" t="s">
-        <v>112</v>
-      </c>
-      <c r="G59" t="s">
-        <v>111</v>
-      </c>
-      <c r="I59" t="s">
-        <v>118</v>
-      </c>
-      <c r="K59" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>11</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60" s="1">
+        <f>DATEVALUE("2021-01-03")+B60+(A60-1)*7</f>
+        <v>44272</v>
+      </c>
+      <c r="D60" t="s">
+        <v>101</v>
+      </c>
+      <c r="E60">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>11</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" s="1">
+        <f>DATEVALUE("2021-01-03")+B61+(A61-1)*7</f>
+        <v>44273</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>11</v>
+      </c>
+      <c r="G61" t="s">
+        <v>52</v>
+      </c>
+      <c r="J61" t="s">
+        <v>72</v>
+      </c>
+      <c r="K61" t="s">
         <v>33</v>
       </c>
-      <c r="M59" t="s">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>11</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62" s="1">
+        <f>DATEVALUE("2021-01-03")+B62+(A62-1)*7</f>
+        <v>44274</v>
+      </c>
+      <c r="D62" t="s">
+        <v>102</v>
+      </c>
+      <c r="E62">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>12</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1">
+        <f>DATEVALUE("2021-01-03")+B63+(A63-1)*7</f>
+        <v>44277</v>
+      </c>
+      <c r="D63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>12</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1">
+        <f>DATEVALUE("2021-01-03")+B64+(A64-1)*7</f>
+        <v>44277</v>
+      </c>
+      <c r="D64" t="s">
+        <v>103</v>
+      </c>
+      <c r="E64">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>12</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65" s="1">
+        <f>DATEVALUE("2021-01-03")+B65+(A65-1)*7</f>
+        <v>44279</v>
+      </c>
+      <c r="D65" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>12</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66" s="1">
+        <f>DATEVALUE("2021-01-03")+B66+(A66-1)*7</f>
+        <v>44279</v>
+      </c>
+      <c r="D66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>12</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67" s="1">
+        <f>DATEVALUE("2021-01-03")+B67+(A67-1)*7</f>
+        <v>44280</v>
+      </c>
+      <c r="D67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" t="s">
+        <v>52</v>
+      </c>
+      <c r="J67" t="s">
+        <v>73</v>
+      </c>
+      <c r="K67" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>12</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68" s="1">
+        <f>DATEVALUE("2021-01-03")+B68+(A68-1)*7</f>
+        <v>44281</v>
+      </c>
+      <c r="D68" t="s">
+        <v>105</v>
+      </c>
+      <c r="E68">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>13</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" s="1">
+        <f>DATEVALUE("2021-01-03")+B69+(A69-1)*7</f>
+        <v>44284</v>
+      </c>
+      <c r="D69" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>13</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70" s="1">
+        <f>DATEVALUE("2021-01-03")+B70+(A70-1)*7</f>
+        <v>44285</v>
+      </c>
+      <c r="D70" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>3</v>
-      </c>
-      <c r="B60">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>13</v>
+      </c>
+      <c r="B71">
+        <v>3</v>
+      </c>
+      <c r="C71" s="1">
+        <f>DATEVALUE("2021-01-03")+B71+(A71-1)*7</f>
+        <v>44286</v>
+      </c>
+      <c r="D71" t="s">
+        <v>107</v>
+      </c>
+      <c r="E71">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>13</v>
+      </c>
+      <c r="B72">
+        <v>4</v>
+      </c>
+      <c r="C72" s="1">
+        <f>DATEVALUE("2021-01-03")+B72+(A72-1)*7</f>
+        <v>44287</v>
+      </c>
+      <c r="D72" t="s">
+        <v>51</v>
+      </c>
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" t="s">
+        <v>52</v>
+      </c>
+      <c r="J72" t="s">
+        <v>48</v>
+      </c>
+      <c r="K72" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>14</v>
+      </c>
+      <c r="B73">
         <v>2</v>
       </c>
-      <c r="C60" s="1">
-        <f t="shared" si="1"/>
-        <v>44215</v>
-      </c>
-      <c r="D60" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61">
+      <c r="C73" s="1">
+        <f>DATEVALUE("2021-01-03")+B73+(A73-1)*7</f>
+        <v>44292</v>
+      </c>
+      <c r="D73" t="s">
+        <v>53</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" t="s">
+        <v>52</v>
+      </c>
+      <c r="J73" t="s">
+        <v>49</v>
+      </c>
+      <c r="K73" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>14</v>
+      </c>
+      <c r="B74">
+        <v>3</v>
+      </c>
+      <c r="C74" s="1">
+        <f>DATEVALUE("2021-01-03")+B74+(A74-1)*7</f>
+        <v>44293</v>
+      </c>
+      <c r="D74" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>14</v>
+      </c>
+      <c r="B75">
         <v>5</v>
       </c>
-      <c r="B61">
-        <v>2</v>
-      </c>
-      <c r="C61" s="1">
-        <f t="shared" si="1"/>
-        <v>44229</v>
-      </c>
-      <c r="D61" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>6</v>
-      </c>
-      <c r="B62">
-        <v>2</v>
-      </c>
-      <c r="C62" s="1">
-        <f t="shared" si="1"/>
-        <v>44236</v>
-      </c>
-      <c r="D62" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>9</v>
-      </c>
-      <c r="B63">
-        <v>2</v>
-      </c>
-      <c r="C63" s="1">
-        <f t="shared" ref="C63:C75" si="2">DATEVALUE("2021-01-03")+B63+(A63-1)*7</f>
-        <v>44257</v>
-      </c>
-      <c r="D63" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>11</v>
-      </c>
-      <c r="B64">
-        <v>2</v>
-      </c>
-      <c r="C64" s="1">
-        <f t="shared" si="2"/>
-        <v>44271</v>
-      </c>
-      <c r="D64" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>13</v>
-      </c>
-      <c r="B65">
-        <v>2</v>
-      </c>
-      <c r="C65" s="1">
-        <f t="shared" si="2"/>
-        <v>44285</v>
-      </c>
-      <c r="D65" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>2</v>
-      </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66" s="1">
-        <f t="shared" si="2"/>
-        <v>44207</v>
-      </c>
-      <c r="D66" t="s">
-        <v>139</v>
-      </c>
-      <c r="F66" t="s">
-        <v>123</v>
-      </c>
-      <c r="J66" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>3</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" s="1">
-        <f t="shared" si="2"/>
-        <v>44214</v>
-      </c>
-      <c r="D67" t="s">
-        <v>140</v>
-      </c>
-      <c r="F67" t="s">
-        <v>123</v>
-      </c>
-      <c r="J67" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>4</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68" s="1">
-        <f t="shared" si="2"/>
-        <v>44221</v>
-      </c>
-      <c r="D68" t="s">
-        <v>141</v>
-      </c>
-      <c r="F68" t="s">
-        <v>126</v>
-      </c>
-      <c r="J68" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>5</v>
-      </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" s="1">
-        <f t="shared" si="2"/>
-        <v>44228</v>
-      </c>
-      <c r="D69" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>6</v>
-      </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70" s="1">
-        <f t="shared" si="2"/>
-        <v>44235</v>
-      </c>
-      <c r="D70" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>8</v>
-      </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-      <c r="C71" s="1">
-        <f t="shared" si="2"/>
-        <v>44249</v>
-      </c>
-      <c r="D71" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>9</v>
-      </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72" s="1">
-        <f t="shared" si="2"/>
-        <v>44256</v>
-      </c>
-      <c r="D72" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>10</v>
-      </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
-      <c r="C73" s="1">
-        <f t="shared" si="2"/>
-        <v>44263</v>
-      </c>
-      <c r="D73" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>11</v>
-      </c>
-      <c r="B74">
-        <v>1</v>
-      </c>
-      <c r="C74" s="1">
-        <f t="shared" si="2"/>
-        <v>44270</v>
-      </c>
-      <c r="D74" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>12</v>
-      </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
       <c r="C75" s="1">
-        <f t="shared" si="2"/>
-        <v>44277</v>
+        <f>DATEVALUE("2021-01-03")+B75+(A75-1)*7</f>
+        <v>44295</v>
       </c>
       <c r="D75" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M58">
-    <sortCondition ref="C2:C58"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M75">
+    <sortCondition ref="C2:C75"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Video links. Slides for more lessons.
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DC213E-41D0-654E-B1D5-7EA006716360}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4708BA4-053A-8B4A-8E27-62A3971352FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="-2120" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="175">
   <si>
     <t>Date</t>
   </si>
@@ -535,6 +535,30 @@
   </si>
   <si>
     <t>Tutorial video</t>
+  </si>
+  <si>
+    <t>slides/12-reshaping-data.html</t>
+  </si>
+  <si>
+    <t>slides/13-displaying-tables.html</t>
+  </si>
+  <si>
+    <t>slides/14-getting-help.html</t>
+  </si>
+  <si>
+    <t>#working-models</t>
+  </si>
+  <si>
+    <t>#linear-models</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=e4b8655e-f365-4cc3-a928-acb500115c80</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=06269a4e-4d7d-4b15-b040-acb50001ff35</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=dc5f62e1-a2b1-42f6-bd7d-acb500dc1f74</t>
   </si>
 </sst>
 </file>
@@ -893,10 +917,10 @@
   <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E9" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1737,11 +1761,23 @@
       <c r="F26" t="s">
         <v>8</v>
       </c>
+      <c r="G26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" t="s">
+        <v>19</v>
+      </c>
       <c r="I26" t="s">
         <v>80</v>
       </c>
       <c r="J26" t="s">
         <v>153</v>
+      </c>
+      <c r="K26" t="s">
+        <v>173</v>
+      </c>
+      <c r="L26" t="s">
+        <v>167</v>
       </c>
       <c r="M26" t="s">
         <v>81</v>
@@ -1782,11 +1818,23 @@
       <c r="F28" t="s">
         <v>8</v>
       </c>
+      <c r="G28" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" t="s">
+        <v>19</v>
+      </c>
       <c r="I28" t="s">
         <v>82</v>
       </c>
       <c r="J28" t="s">
         <v>154</v>
+      </c>
+      <c r="K28" t="s">
+        <v>174</v>
+      </c>
+      <c r="L28" t="s">
+        <v>168</v>
       </c>
       <c r="M28" t="s">
         <v>83</v>
@@ -1839,11 +1887,23 @@
       <c r="F30" t="s">
         <v>8</v>
       </c>
+      <c r="G30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
       <c r="I30" t="s">
         <v>21</v>
       </c>
       <c r="J30" t="s">
         <v>156</v>
+      </c>
+      <c r="K30" t="s">
+        <v>172</v>
+      </c>
+      <c r="L30" t="s">
+        <v>169</v>
       </c>
       <c r="M30" t="s">
         <v>157</v>
@@ -1881,6 +1941,12 @@
       <c r="E32">
         <v>15</v>
       </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -1928,6 +1994,12 @@
       </c>
       <c r="E35">
         <v>16</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
revised week 6, new slides
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C712A152-5D21-F24D-98E9-AB40F2B1A8F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75961726-2ADC-444E-84F8-D70135D50162}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28040" yWindow="-2120" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
+    <workbookView xWindow="-28040" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="181">
   <si>
     <t>Date</t>
   </si>
@@ -565,6 +565,18 @@
   </si>
   <si>
     <t>Project teams sign-up deadline</t>
+  </si>
+  <si>
+    <t>slides/15-working-with-models.html</t>
+  </si>
+  <si>
+    <t>slides/16-linear-models.html</t>
+  </si>
+  <si>
+    <t>slides/17-gam-loess.html</t>
+  </si>
+  <si>
+    <t>#smoothing</t>
   </si>
 </sst>
 </file>
@@ -923,10 +935,10 @@
   <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E52" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E19" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
+      <selection pane="bottomRight" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1950,11 +1962,17 @@
       <c r="F32" t="s">
         <v>8</v>
       </c>
+      <c r="H32" t="s">
+        <v>19</v>
+      </c>
       <c r="J32" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1969,7 +1987,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>6</v>
       </c>
@@ -1984,7 +2002,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>6</v>
       </c>
@@ -2004,11 +2022,17 @@
       <c r="F35" t="s">
         <v>8</v>
       </c>
+      <c r="H35" t="s">
+        <v>19</v>
+      </c>
       <c r="J35" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>6</v>
       </c>
@@ -2035,7 +2059,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>6</v>
       </c>
@@ -2052,8 +2076,20 @@
       <c r="E37">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" t="s">
+        <v>180</v>
+      </c>
+      <c r="L37" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>8</v>
       </c>
@@ -2068,7 +2104,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2086,7 +2122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2104,7 +2140,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>8</v>
       </c>
@@ -2119,7 +2155,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>8</v>
       </c>
@@ -2146,7 +2182,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>8</v>
       </c>
@@ -2164,7 +2200,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>9</v>
       </c>
@@ -2179,7 +2215,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>9</v>
       </c>
@@ -2197,7 +2233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>9</v>
       </c>
@@ -2212,7 +2248,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>9</v>
       </c>
@@ -2230,7 +2266,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Updated week 6, formatting, slides
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75961726-2ADC-444E-84F8-D70135D50162}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F6B89-45B7-7642-BFD8-6AA6AA8F4642}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="191">
   <si>
     <t>Date</t>
   </si>
@@ -300,9 +300,6 @@
     <t>Plotting facets</t>
   </si>
   <si>
-    <t>Formatting tables</t>
-  </si>
-  <si>
     <t>Working with models</t>
   </si>
   <si>
@@ -577,6 +574,39 @@
   </si>
   <si>
     <t>#smoothing</t>
+  </si>
+  <si>
+    <t>Bonus taks</t>
+  </si>
+  <si>
+    <t>Task 9</t>
+  </si>
+  <si>
+    <t>Task 10</t>
+  </si>
+  <si>
+    <t>Collaboration with GitHub</t>
+  </si>
+  <si>
+    <t>#task-b7</t>
+  </si>
+  <si>
+    <t>#task-9</t>
+  </si>
+  <si>
+    <t>#task-10</t>
+  </si>
+  <si>
+    <t>#collaboration</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>#assignment-3</t>
+  </si>
+  <si>
+    <t>#assignment-2</t>
   </si>
 </sst>
 </file>
@@ -935,10 +965,10 @@
   <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E19" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J35" sqref="J35"/>
+      <selection pane="bottomRight" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1129,7 +1159,7 @@
         <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L5" t="s">
         <v>37</v>
@@ -1150,13 +1180,13 @@
         <v>44207</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" t="s">
         <v>117</v>
-      </c>
-      <c r="J6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1210,7 +1240,7 @@
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K8" t="s">
         <v>33</v>
@@ -1249,7 +1279,7 @@
         <v>41</v>
       </c>
       <c r="K9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L9" t="s">
         <v>42</v>
@@ -1291,7 +1321,7 @@
         <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L10" t="s">
         <v>47</v>
@@ -1339,13 +1369,13 @@
         <v>44214</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1381,7 +1411,7 @@
         <v>55</v>
       </c>
       <c r="K13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L13" t="s">
         <v>56</v>
@@ -1423,13 +1453,13 @@
         <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1444,19 +1474,19 @@
         <v>44215</v>
       </c>
       <c r="D15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" t="s">
         <v>111</v>
-      </c>
-      <c r="G15" t="s">
-        <v>110</v>
-      </c>
-      <c r="I15" t="s">
-        <v>112</v>
       </c>
       <c r="K15" t="s">
         <v>33</v>
       </c>
       <c r="M15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1471,7 +1501,7 @@
         <v>44214</v>
       </c>
       <c r="D16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1507,13 +1537,13 @@
         <v>59</v>
       </c>
       <c r="K17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1573,13 +1603,13 @@
         <v>76</v>
       </c>
       <c r="J19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M19" t="s">
         <v>77</v>
@@ -1597,19 +1627,19 @@
         <v>44221</v>
       </c>
       <c r="D20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J20" t="s">
         <v>57</v>
       </c>
       <c r="K20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1642,13 +1672,13 @@
         <v>78</v>
       </c>
       <c r="J21" t="s">
+        <v>148</v>
+      </c>
+      <c r="K21" t="s">
+        <v>164</v>
+      </c>
+      <c r="L21" t="s">
         <v>149</v>
-      </c>
-      <c r="K21" t="s">
-        <v>165</v>
-      </c>
-      <c r="L21" t="s">
-        <v>150</v>
       </c>
       <c r="M21" t="s">
         <v>79</v>
@@ -1666,7 +1696,7 @@
         <v>44223</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F22" t="s">
         <v>63</v>
@@ -1732,16 +1762,16 @@
         <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1756,7 +1786,7 @@
         <v>44228</v>
       </c>
       <c r="D25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1789,13 +1819,13 @@
         <v>80</v>
       </c>
       <c r="J26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M26" t="s">
         <v>81</v>
@@ -1813,7 +1843,13 @@
         <v>44229</v>
       </c>
       <c r="D27" t="s">
-        <v>159</v>
+        <v>158</v>
+      </c>
+      <c r="I27" t="s">
+        <v>188</v>
+      </c>
+      <c r="M27" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -1828,7 +1864,7 @@
         <v>44230</v>
       </c>
       <c r="D28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E28">
         <v>13</v>
@@ -1846,13 +1882,13 @@
         <v>82</v>
       </c>
       <c r="J28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M28" t="s">
         <v>83</v>
@@ -1897,7 +1933,7 @@
         <v>44231</v>
       </c>
       <c r="D30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E30">
         <v>14</v>
@@ -1915,16 +1951,16 @@
         <v>21</v>
       </c>
       <c r="J30" t="s">
+        <v>155</v>
+      </c>
+      <c r="K30" t="s">
+        <v>171</v>
+      </c>
+      <c r="L30" t="s">
+        <v>168</v>
+      </c>
+      <c r="M30" t="s">
         <v>156</v>
-      </c>
-      <c r="K30" t="s">
-        <v>172</v>
-      </c>
-      <c r="L30" t="s">
-        <v>169</v>
-      </c>
-      <c r="M30" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -1939,7 +1975,7 @@
         <v>44235</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -1954,7 +1990,7 @@
         <v>44235</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E32">
         <v>15</v>
@@ -1962,17 +1998,26 @@
       <c r="F32" t="s">
         <v>8</v>
       </c>
+      <c r="G32" t="s">
+        <v>3</v>
+      </c>
       <c r="H32" t="s">
         <v>19</v>
       </c>
+      <c r="I32" t="s">
+        <v>180</v>
+      </c>
       <c r="J32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L32" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+      <c r="M32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1984,10 +2029,16 @@
         <v>44236</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="I33" t="s">
+        <v>188</v>
+      </c>
+      <c r="M33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>6</v>
       </c>
@@ -1999,10 +2050,10 @@
         <v>44237</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>6</v>
       </c>
@@ -2014,7 +2065,7 @@
         <v>44237</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E35">
         <v>16</v>
@@ -2022,17 +2073,26 @@
       <c r="F35" t="s">
         <v>8</v>
       </c>
+      <c r="G35" t="s">
+        <v>3</v>
+      </c>
       <c r="H35" t="s">
         <v>19</v>
       </c>
+      <c r="I35" t="s">
+        <v>181</v>
+      </c>
       <c r="J35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L35" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+      <c r="M35" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>6</v>
       </c>
@@ -2059,7 +2119,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>6</v>
       </c>
@@ -2071,7 +2131,7 @@
         <v>44239</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E37">
         <v>17</v>
@@ -2079,17 +2139,26 @@
       <c r="F37" t="s">
         <v>8</v>
       </c>
+      <c r="G37" t="s">
+        <v>3</v>
+      </c>
       <c r="H37" t="s">
         <v>19</v>
       </c>
+      <c r="I37" t="s">
+        <v>182</v>
+      </c>
       <c r="J37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L37" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+      <c r="M37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>8</v>
       </c>
@@ -2101,10 +2170,10 @@
         <v>44249</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2116,13 +2185,19 @@
         <v>44249</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>183</v>
       </c>
       <c r="E39">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2134,13 +2209,13 @@
         <v>44251</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E40">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>8</v>
       </c>
@@ -2152,10 +2227,10 @@
         <v>44251</v>
       </c>
       <c r="D41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>8</v>
       </c>
@@ -2182,7 +2257,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>8</v>
       </c>
@@ -2194,13 +2269,13 @@
         <v>44253</v>
       </c>
       <c r="D43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E43">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>9</v>
       </c>
@@ -2212,10 +2287,10 @@
         <v>44256</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>9</v>
       </c>
@@ -2227,13 +2302,13 @@
         <v>44256</v>
       </c>
       <c r="D45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E45">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>9</v>
       </c>
@@ -2245,10 +2320,10 @@
         <v>44257</v>
       </c>
       <c r="D46" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>9</v>
       </c>
@@ -2260,13 +2335,13 @@
         <v>44258</v>
       </c>
       <c r="D47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E47">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>9</v>
       </c>
@@ -2305,7 +2380,7 @@
         <v>44260</v>
       </c>
       <c r="D49" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E49">
         <v>23</v>
@@ -2323,7 +2398,7 @@
         <v>44263</v>
       </c>
       <c r="D50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -2338,7 +2413,7 @@
         <v>44263</v>
       </c>
       <c r="D51" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E51">
         <v>24</v>
@@ -2356,7 +2431,7 @@
         <v>44265</v>
       </c>
       <c r="D52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E52">
         <v>25</v>
@@ -2374,7 +2449,7 @@
         <v>44265</v>
       </c>
       <c r="D53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2416,7 +2491,7 @@
         <v>44267</v>
       </c>
       <c r="D55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E55">
         <v>26</v>
@@ -2434,7 +2509,7 @@
         <v>44267</v>
       </c>
       <c r="D56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -2449,7 +2524,7 @@
         <v>44270</v>
       </c>
       <c r="D57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -2464,7 +2539,7 @@
         <v>44270</v>
       </c>
       <c r="D58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E58">
         <v>27</v>
@@ -2482,7 +2557,7 @@
         <v>44271</v>
       </c>
       <c r="D59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -2497,7 +2572,7 @@
         <v>44272</v>
       </c>
       <c r="D60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E60">
         <v>28</v>
@@ -2542,7 +2617,7 @@
         <v>44274</v>
       </c>
       <c r="D62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E62">
         <v>29</v>
@@ -2560,7 +2635,7 @@
         <v>44277</v>
       </c>
       <c r="D63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -2575,7 +2650,7 @@
         <v>44277</v>
       </c>
       <c r="D64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E64">
         <v>30</v>
@@ -2593,7 +2668,7 @@
         <v>44279</v>
       </c>
       <c r="D65" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E65">
         <v>31</v>
@@ -2611,7 +2686,7 @@
         <v>44279</v>
       </c>
       <c r="D66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -2653,7 +2728,7 @@
         <v>44281</v>
       </c>
       <c r="D68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E68">
         <v>32</v>
@@ -2671,7 +2746,7 @@
         <v>44284</v>
       </c>
       <c r="D69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E69">
         <v>33</v>
@@ -2689,7 +2764,7 @@
         <v>44285</v>
       </c>
       <c r="D70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2704,7 +2779,7 @@
         <v>44286</v>
       </c>
       <c r="D71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E71">
         <v>34</v>
@@ -2776,7 +2851,7 @@
         <v>44293</v>
       </c>
       <c r="D74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -2791,7 +2866,7 @@
         <v>44295</v>
       </c>
       <c r="D75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -2806,7 +2881,7 @@
         <v>44249</v>
       </c>
       <c r="D76" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -2821,7 +2896,7 @@
         <v>44253</v>
       </c>
       <c r="D77" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Links to videos for week 6
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F6B89-45B7-7642-BFD8-6AA6AA8F4642}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A93818-9944-EF4E-8E83-F521027D2FFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="194">
   <si>
     <t>Date</t>
   </si>
@@ -607,6 +607,15 @@
   </si>
   <si>
     <t>#assignment-2</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=71abc712-222a-45b1-8dff-acc7013ceb32</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=b241bfa7-de23-49bd-905b-acc70142c214</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=fbeef455-8789-42b9-92df-acc7014943ca</t>
   </si>
 </sst>
 </file>
@@ -968,7 +977,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I34" sqref="I34"/>
+      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2010,6 +2019,9 @@
       <c r="J32" t="s">
         <v>169</v>
       </c>
+      <c r="K32" t="s">
+        <v>191</v>
+      </c>
       <c r="L32" t="s">
         <v>176</v>
       </c>
@@ -2085,6 +2097,9 @@
       <c r="J35" t="s">
         <v>170</v>
       </c>
+      <c r="K35" t="s">
+        <v>192</v>
+      </c>
       <c r="L35" t="s">
         <v>177</v>
       </c>
@@ -2150,6 +2165,9 @@
       </c>
       <c r="J37" t="s">
         <v>179</v>
+      </c>
+      <c r="K37" t="s">
+        <v>193</v>
       </c>
       <c r="L37" t="s">
         <v>178</v>

</xml_diff>

<commit_message>
Updated for week 7
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DDDB71-967D-804B-9637-BB1941407A34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FF2DC5-3ABC-6142-8BBE-3A5A583312F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="203">
   <si>
     <t>Date</t>
   </si>
@@ -576,9 +576,6 @@
     <t>#smoothing</t>
   </si>
   <si>
-    <t>Bonus taks</t>
-  </si>
-  <si>
     <t>Task 9</t>
   </si>
   <si>
@@ -628,6 +625,24 @@
   </si>
   <si>
     <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=cd65821d-465b-45b1-a052-acc90145c93d</t>
+  </si>
+  <si>
+    <t>slides/19-PCA.html</t>
+  </si>
+  <si>
+    <t>#task-b8</t>
+  </si>
+  <si>
+    <t>#task-12</t>
+  </si>
+  <si>
+    <t>Task 12</t>
+  </si>
+  <si>
+    <t>#mds</t>
+  </si>
+  <si>
+    <t>#PCA</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1004,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E16" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K39" sqref="K39"/>
+      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1867,10 +1882,10 @@
         <v>158</v>
       </c>
       <c r="I27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -2026,19 +2041,19 @@
         <v>19</v>
       </c>
       <c r="I32" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
       <c r="J32" t="s">
         <v>169</v>
       </c>
       <c r="K32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L32" t="s">
         <v>176</v>
       </c>
       <c r="M32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -2056,10 +2071,10 @@
         <v>160</v>
       </c>
       <c r="I33" t="s">
+        <v>187</v>
+      </c>
+      <c r="M33" t="s">
         <v>188</v>
-      </c>
-      <c r="M33" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -2104,19 +2119,19 @@
         <v>19</v>
       </c>
       <c r="I35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J35" t="s">
         <v>170</v>
       </c>
       <c r="K35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L35" t="s">
         <v>177</v>
       </c>
       <c r="M35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -2173,19 +2188,19 @@
         <v>19</v>
       </c>
       <c r="I37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J37" t="s">
         <v>179</v>
       </c>
       <c r="K37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L37" t="s">
         <v>178</v>
       </c>
       <c r="M37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -2215,7 +2230,7 @@
         <v>44249</v>
       </c>
       <c r="D39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E39">
         <v>18</v>
@@ -2230,19 +2245,19 @@
         <v>19</v>
       </c>
       <c r="I39" t="s">
+        <v>193</v>
+      </c>
+      <c r="J39" t="s">
+        <v>186</v>
+      </c>
+      <c r="K39" t="s">
+        <v>196</v>
+      </c>
+      <c r="L39" t="s">
+        <v>195</v>
+      </c>
+      <c r="M39" t="s">
         <v>194</v>
-      </c>
-      <c r="J39" t="s">
-        <v>187</v>
-      </c>
-      <c r="K39" t="s">
-        <v>197</v>
-      </c>
-      <c r="L39" t="s">
-        <v>196</v>
-      </c>
-      <c r="M39" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -2262,6 +2277,24 @@
       <c r="E40">
         <v>19</v>
       </c>
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" t="s">
+        <v>202</v>
+      </c>
+      <c r="L40" t="s">
+        <v>197</v>
+      </c>
+      <c r="M40" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -2321,6 +2354,18 @@
       </c>
       <c r="E43">
         <v>20</v>
+      </c>
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+      <c r="I43" t="s">
+        <v>200</v>
+      </c>
+      <c r="J43" t="s">
+        <v>201</v>
+      </c>
+      <c r="M43" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
More updates. Week 8 or so
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FF2DC5-3ABC-6142-8BBE-3A5A583312F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C05598-F6FE-FD4E-807A-2A6788A7C070}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -420,12 +420,6 @@
     <t>Tasks 9 and 10 due at 9 am</t>
   </si>
   <si>
-    <t>Tasks 11 and 12 due at 9 am</t>
-  </si>
-  <si>
-    <t>Tasks 13 and 14 due at 9 am</t>
-  </si>
-  <si>
     <t>Tasks 15 and 16 due at 9 am</t>
   </si>
   <si>
@@ -643,6 +637,12 @@
   </si>
   <si>
     <t>#PCA</t>
+  </si>
+  <si>
+    <t>Task 11 due at 9 am</t>
+  </si>
+  <si>
+    <t>Tasks 12, 13 and 14 due at 9 am</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +1001,10 @@
   <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E16" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E28" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,7 +1216,7 @@
         <v>44207</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F6" t="s">
         <v>116</v>
@@ -1405,7 +1405,7 @@
         <v>44214</v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F12" t="s">
         <v>116</v>
@@ -1489,13 +1489,13 @@
         <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1522,7 +1522,7 @@
         <v>33</v>
       </c>
       <c r="M15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1537,7 +1537,7 @@
         <v>44214</v>
       </c>
       <c r="D16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1573,13 +1573,13 @@
         <v>59</v>
       </c>
       <c r="K17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1639,13 +1639,13 @@
         <v>76</v>
       </c>
       <c r="J19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M19" t="s">
         <v>77</v>
@@ -1663,19 +1663,19 @@
         <v>44221</v>
       </c>
       <c r="D20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F20" t="s">
         <v>119</v>
       </c>
       <c r="G20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J20" t="s">
         <v>57</v>
       </c>
       <c r="K20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1708,13 +1708,13 @@
         <v>78</v>
       </c>
       <c r="J21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M21" t="s">
         <v>79</v>
@@ -1798,16 +1798,16 @@
         <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1822,7 +1822,7 @@
         <v>44228</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1855,13 +1855,13 @@
         <v>80</v>
       </c>
       <c r="J26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="M26" t="s">
         <v>81</v>
@@ -1879,13 +1879,13 @@
         <v>44229</v>
       </c>
       <c r="D27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I27" t="s">
+        <v>185</v>
+      </c>
+      <c r="M27" t="s">
         <v>187</v>
-      </c>
-      <c r="M27" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -1900,7 +1900,7 @@
         <v>44230</v>
       </c>
       <c r="D28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E28">
         <v>13</v>
@@ -1918,13 +1918,13 @@
         <v>82</v>
       </c>
       <c r="J28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M28" t="s">
         <v>83</v>
@@ -1969,7 +1969,7 @@
         <v>44231</v>
       </c>
       <c r="D30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E30">
         <v>14</v>
@@ -1987,16 +1987,16 @@
         <v>21</v>
       </c>
       <c r="J30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -2044,16 +2044,16 @@
         <v>21</v>
       </c>
       <c r="J32" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="M32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -2068,13 +2068,13 @@
         <v>44236</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I33" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -2119,19 +2119,19 @@
         <v>19</v>
       </c>
       <c r="I35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K35" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M35" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -2188,19 +2188,19 @@
         <v>19</v>
       </c>
       <c r="I37" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J37" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L37" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M37" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -2208,11 +2208,11 @@
         <v>8</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="1"/>
-        <v>44249</v>
+        <v>44251</v>
       </c>
       <c r="D38" t="s">
         <v>127</v>
@@ -2230,7 +2230,7 @@
         <v>44249</v>
       </c>
       <c r="D39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E39">
         <v>18</v>
@@ -2245,19 +2245,19 @@
         <v>19</v>
       </c>
       <c r="I39" t="s">
+        <v>191</v>
+      </c>
+      <c r="J39" t="s">
+        <v>184</v>
+      </c>
+      <c r="K39" t="s">
+        <v>194</v>
+      </c>
+      <c r="L39" t="s">
         <v>193</v>
       </c>
-      <c r="J39" t="s">
-        <v>186</v>
-      </c>
-      <c r="K39" t="s">
-        <v>196</v>
-      </c>
-      <c r="L39" t="s">
-        <v>195</v>
-      </c>
       <c r="M39" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -2287,13 +2287,13 @@
         <v>21</v>
       </c>
       <c r="J40" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L40" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M40" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -2359,13 +2359,13 @@
         <v>8</v>
       </c>
       <c r="I43" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J43" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M43" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
@@ -2380,7 +2380,7 @@
         <v>44256</v>
       </c>
       <c r="D44" t="s">
-        <v>128</v>
+        <v>201</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -2413,7 +2413,7 @@
         <v>44257</v>
       </c>
       <c r="D46" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -2491,7 +2491,7 @@
         <v>44263</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -2617,7 +2617,7 @@
         <v>44270</v>
       </c>
       <c r="D57" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -2650,7 +2650,7 @@
         <v>44271</v>
       </c>
       <c r="D59" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -2728,7 +2728,7 @@
         <v>44277</v>
       </c>
       <c r="D63" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -2857,7 +2857,7 @@
         <v>44285</v>
       </c>
       <c r="D70" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2974,7 +2974,7 @@
         <v>44249</v>
       </c>
       <c r="D76" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -2989,7 +2989,7 @@
         <v>44256</v>
       </c>
       <c r="D77" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised schedule to end of course. Some content updates.
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C05598-F6FE-FD4E-807A-2A6788A7C070}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FB3A2A-F78D-BC4C-B16C-6250D2099908}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28040" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
+    <workbookView xWindow="-71820" yWindow="2460" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="230">
   <si>
     <t>Date</t>
   </si>
@@ -324,39 +324,15 @@
     <t>Slide presentations</t>
   </si>
   <si>
-    <t>Tidy data</t>
-  </si>
-  <si>
-    <t>Validating data</t>
-  </si>
-  <si>
-    <t>Finding and describing data</t>
-  </si>
-  <si>
     <t>Making maps</t>
   </si>
   <si>
-    <t>Chloropleths and non-maps</t>
-  </si>
-  <si>
-    <t>Working with factors</t>
-  </si>
-  <si>
     <t>Themes</t>
   </si>
   <si>
-    <t>Annotations</t>
-  </si>
-  <si>
     <t>Graphics output</t>
   </si>
   <si>
-    <t>Working with dates</t>
-  </si>
-  <si>
-    <t>Topic TBA</t>
-  </si>
-  <si>
     <t>Project proposal due</t>
   </si>
   <si>
@@ -643,6 +619,111 @@
   </si>
   <si>
     <t>Tasks 12, 13 and 14 due at 9 am</t>
+  </si>
+  <si>
+    <t>Finding data</t>
+  </si>
+  <si>
+    <t>Using colour</t>
+  </si>
+  <si>
+    <t>Factors and Dates</t>
+  </si>
+  <si>
+    <t>More about maps</t>
+  </si>
+  <si>
+    <t>Alternatives to maps</t>
+  </si>
+  <si>
+    <t>Cleaning and validating data</t>
+  </si>
+  <si>
+    <t>#slides</t>
+  </si>
+  <si>
+    <t>#mapping-1</t>
+  </si>
+  <si>
+    <t>#k-means</t>
+  </si>
+  <si>
+    <t>#factors-dates</t>
+  </si>
+  <si>
+    <t>#colour</t>
+  </si>
+  <si>
+    <t>Dynamic graphics</t>
+  </si>
+  <si>
+    <t>Reconstructing a visualization</t>
+  </si>
+  <si>
+    <t>#theme</t>
+  </si>
+  <si>
+    <t>slides/35-step-by-step.html</t>
+  </si>
+  <si>
+    <t>#output-files</t>
+  </si>
+  <si>
+    <t>Task 13</t>
+  </si>
+  <si>
+    <t>#task-13</t>
+  </si>
+  <si>
+    <t>#task-14</t>
+  </si>
+  <si>
+    <t>Task 14</t>
+  </si>
+  <si>
+    <t>#task-b9</t>
+  </si>
+  <si>
+    <t>Task 15</t>
+  </si>
+  <si>
+    <t>Task 16</t>
+  </si>
+  <si>
+    <t>#task-15</t>
+  </si>
+  <si>
+    <t>#task-16</t>
+  </si>
+  <si>
+    <t>Task 17</t>
+  </si>
+  <si>
+    <t>Task 18</t>
+  </si>
+  <si>
+    <t>#task-b10</t>
+  </si>
+  <si>
+    <t>#task-17</t>
+  </si>
+  <si>
+    <t>#task-18</t>
+  </si>
+  <si>
+    <t>Task 19</t>
+  </si>
+  <si>
+    <t>Task 20</t>
+  </si>
+  <si>
+    <t>#task-20</t>
+  </si>
+  <si>
+    <t>#task-19</t>
+  </si>
+  <si>
+    <t>#task-b11</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +1082,10 @@
   <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E28" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1195,7 +1276,7 @@
         <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="L5" t="s">
         <v>37</v>
@@ -1216,13 +1297,13 @@
         <v>44207</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F6" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="J6" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1276,7 +1357,7 @@
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="K8" t="s">
         <v>33</v>
@@ -1315,7 +1396,7 @@
         <v>41</v>
       </c>
       <c r="K9" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="L9" t="s">
         <v>42</v>
@@ -1357,7 +1438,7 @@
         <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="L10" t="s">
         <v>47</v>
@@ -1405,13 +1486,13 @@
         <v>44214</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="J12" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1447,7 +1528,7 @@
         <v>55</v>
       </c>
       <c r="K13" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L13" t="s">
         <v>56</v>
@@ -1489,13 +1570,13 @@
         <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="L14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="M14" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1510,19 +1591,19 @@
         <v>44215</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G15" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I15" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K15" t="s">
         <v>33</v>
       </c>
       <c r="M15" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1537,7 +1618,7 @@
         <v>44214</v>
       </c>
       <c r="D16" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1573,13 +1654,13 @@
         <v>59</v>
       </c>
       <c r="K17" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="L17" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="M17" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1639,13 +1720,13 @@
         <v>76</v>
       </c>
       <c r="J19" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="K19" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="L19" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="M19" t="s">
         <v>77</v>
@@ -1663,19 +1744,19 @@
         <v>44221</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G20" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="J20" t="s">
         <v>57</v>
       </c>
       <c r="K20" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1708,13 +1789,13 @@
         <v>78</v>
       </c>
       <c r="J21" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="K21" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="L21" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="M21" t="s">
         <v>79</v>
@@ -1732,7 +1813,7 @@
         <v>44223</v>
       </c>
       <c r="D22" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F22" t="s">
         <v>63</v>
@@ -1798,16 +1879,16 @@
         <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="K24" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="L24" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="M24" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1822,7 +1903,7 @@
         <v>44228</v>
       </c>
       <c r="D25" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1855,13 +1936,13 @@
         <v>80</v>
       </c>
       <c r="J26" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="K26" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="L26" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="M26" t="s">
         <v>81</v>
@@ -1879,13 +1960,13 @@
         <v>44229</v>
       </c>
       <c r="D27" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I27" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="M27" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -1900,7 +1981,7 @@
         <v>44230</v>
       </c>
       <c r="D28" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E28">
         <v>13</v>
@@ -1918,13 +1999,13 @@
         <v>82</v>
       </c>
       <c r="J28" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="K28" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="L28" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="M28" t="s">
         <v>83</v>
@@ -1969,7 +2050,7 @@
         <v>44231</v>
       </c>
       <c r="D30" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E30">
         <v>14</v>
@@ -1987,16 +2068,16 @@
         <v>21</v>
       </c>
       <c r="J30" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="K30" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="L30" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="M30" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -2007,11 +2088,11 @@
         <v>1</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="0"/>
+        <f>DATEVALUE("2021-01-03")+B31+(A31-1)*7</f>
         <v>44235</v>
       </c>
       <c r="D31" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -2022,7 +2103,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="0"/>
+        <f>DATEVALUE("2021-01-03")+B32+(A32-1)*7</f>
         <v>44235</v>
       </c>
       <c r="D32" t="s">
@@ -2044,16 +2125,16 @@
         <v>21</v>
       </c>
       <c r="J32" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="K32" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="L32" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="M32" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -2064,17 +2145,17 @@
         <v>2</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="0"/>
+        <f>DATEVALUE("2021-01-03")+B33+(A33-1)*7</f>
         <v>44236</v>
       </c>
       <c r="D33" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="I33" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="M33" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -2085,11 +2166,11 @@
         <v>3</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" ref="C34:C65" si="1">DATEVALUE("2021-01-03")+B34+(A34-1)*7</f>
+        <f>DATEVALUE("2021-01-03")+B34+(A34-1)*7</f>
         <v>44237</v>
       </c>
       <c r="D34" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -2100,7 +2181,7 @@
         <v>3</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" si="1"/>
+        <f>DATEVALUE("2021-01-03")+B35+(A35-1)*7</f>
         <v>44237</v>
       </c>
       <c r="D35" t="s">
@@ -2119,19 +2200,19 @@
         <v>19</v>
       </c>
       <c r="I35" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="J35" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="K35" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="L35" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="M35" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -2142,7 +2223,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" si="1"/>
+        <f>DATEVALUE("2021-01-03")+B36+(A36-1)*7</f>
         <v>44238</v>
       </c>
       <c r="D36" t="s">
@@ -2169,7 +2250,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" si="1"/>
+        <f>DATEVALUE("2021-01-03")+B37+(A37-1)*7</f>
         <v>44239</v>
       </c>
       <c r="D37" t="s">
@@ -2188,19 +2269,19 @@
         <v>19</v>
       </c>
       <c r="I37" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="J37" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="K37" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="L37" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="M37" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -2208,14 +2289,41 @@
         <v>8</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" si="1"/>
-        <v>44251</v>
+        <f>DATEVALUE("2021-01-03")+B38+(A38-1)*7</f>
+        <v>44249</v>
       </c>
       <c r="D38" t="s">
-        <v>127</v>
+        <v>172</v>
+      </c>
+      <c r="E38">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>3</v>
+      </c>
+      <c r="H38" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" t="s">
+        <v>183</v>
+      </c>
+      <c r="J38" t="s">
+        <v>176</v>
+      </c>
+      <c r="K38" t="s">
+        <v>186</v>
+      </c>
+      <c r="L38" t="s">
+        <v>185</v>
+      </c>
+      <c r="M38" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
@@ -2226,38 +2334,11 @@
         <v>1</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" si="1"/>
+        <f>DATEVALUE("2021-01-03")+B39+(A39-1)*7</f>
         <v>44249</v>
       </c>
       <c r="D39" t="s">
-        <v>180</v>
-      </c>
-      <c r="E39">
-        <v>18</v>
-      </c>
-      <c r="F39" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" t="s">
-        <v>3</v>
-      </c>
-      <c r="H39" t="s">
-        <v>19</v>
-      </c>
-      <c r="I39" t="s">
-        <v>191</v>
-      </c>
-      <c r="J39" t="s">
-        <v>184</v>
-      </c>
-      <c r="K39" t="s">
-        <v>194</v>
-      </c>
-      <c r="L39" t="s">
-        <v>193</v>
-      </c>
-      <c r="M39" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -2268,32 +2349,11 @@
         <v>3</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" si="1"/>
+        <f>DATEVALUE("2021-01-03")+B40+(A40-1)*7</f>
         <v>44251</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
-      </c>
-      <c r="E40">
-        <v>19</v>
-      </c>
-      <c r="F40" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" t="s">
-        <v>19</v>
-      </c>
-      <c r="I40" t="s">
-        <v>21</v>
-      </c>
-      <c r="J40" t="s">
-        <v>200</v>
-      </c>
-      <c r="L40" t="s">
-        <v>195</v>
-      </c>
-      <c r="M40" t="s">
-        <v>196</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -2304,11 +2364,23 @@
         <v>3</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" si="1"/>
+        <f>DATEVALUE("2021-01-03")+B41+(A41-1)*7</f>
         <v>44251</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>195</v>
+      </c>
+      <c r="E41">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+      <c r="I41" t="s">
+        <v>21</v>
+      </c>
+      <c r="M41" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -2316,26 +2388,14 @@
         <v>8</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" si="1"/>
-        <v>44252</v>
+        <f>DATEVALUE("2021-01-03")+B42+(A42-1)*7</f>
+        <v>44251</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" t="s">
-        <v>52</v>
-      </c>
-      <c r="J42" t="s">
-        <v>69</v>
-      </c>
-      <c r="K42" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -2343,44 +2403,53 @@
         <v>8</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" si="1"/>
-        <v>44253</v>
+        <f>DATEVALUE("2021-01-03")+B43+(A43-1)*7</f>
+        <v>44252</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>8</v>
-      </c>
-      <c r="I43" t="s">
-        <v>198</v>
+        <v>11</v>
+      </c>
+      <c r="G43" t="s">
+        <v>52</v>
       </c>
       <c r="J43" t="s">
-        <v>199</v>
-      </c>
-      <c r="M43" t="s">
-        <v>197</v>
+        <v>69</v>
+      </c>
+      <c r="K43" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" si="1"/>
-        <v>44256</v>
+        <f>DATEVALUE("2021-01-03")+B44+(A44-1)*7</f>
+        <v>44253</v>
       </c>
       <c r="D44" t="s">
-        <v>201</v>
+        <v>94</v>
+      </c>
+      <c r="E44">
+        <v>20</v>
+      </c>
+      <c r="F44" t="s">
+        <v>8</v>
+      </c>
+      <c r="I44" t="s">
+        <v>190</v>
+      </c>
+      <c r="M44" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -2391,14 +2460,32 @@
         <v>1</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" si="1"/>
+        <f>DATEVALUE("2021-01-03")+B45+(A45-1)*7</f>
         <v>44256</v>
       </c>
       <c r="D45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E45">
         <v>21</v>
+      </c>
+      <c r="F45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" t="s">
+        <v>19</v>
+      </c>
+      <c r="I45" t="s">
+        <v>211</v>
+      </c>
+      <c r="J45" t="s">
+        <v>192</v>
+      </c>
+      <c r="L45" t="s">
+        <v>187</v>
+      </c>
+      <c r="M45" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -2406,14 +2493,14 @@
         <v>9</v>
       </c>
       <c r="B46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" si="1"/>
-        <v>44257</v>
+        <f>DATEVALUE("2021-01-03")+B46+(A46-1)*7</f>
+        <v>44256</v>
       </c>
       <c r="D46" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -2421,17 +2508,14 @@
         <v>9</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" si="1"/>
-        <v>44258</v>
+        <f>DATEVALUE("2021-01-03")+B47+(A47-1)*7</f>
+        <v>44256</v>
       </c>
       <c r="D47" t="s">
-        <v>94</v>
-      </c>
-      <c r="E47">
-        <v>22</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -2439,562 +2523,680 @@
         <v>9</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" si="1"/>
-        <v>44259</v>
+        <f>DATEVALUE("2021-01-03")+B48+(A48-1)*7</f>
+        <v>44257</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" t="s">
-        <v>11</v>
-      </c>
-      <c r="G48" t="s">
-        <v>52</v>
-      </c>
-      <c r="J48" t="s">
-        <v>70</v>
-      </c>
-      <c r="K48" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>9</v>
       </c>
       <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49" s="1">
+        <f>DATEVALUE("2021-01-03")+B49+(A49-1)*7</f>
+        <v>44258</v>
+      </c>
+      <c r="D49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E49">
+        <v>22</v>
+      </c>
+      <c r="F49" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>9</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
+        <f>DATEVALUE("2021-01-03")+B50+(A50-1)*7</f>
+        <v>44259</v>
+      </c>
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" t="s">
+        <v>52</v>
+      </c>
+      <c r="J50" t="s">
+        <v>70</v>
+      </c>
+      <c r="K50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51">
         <v>5</v>
       </c>
-      <c r="C49" s="1">
-        <f t="shared" si="1"/>
+      <c r="C51" s="1">
+        <f>DATEVALUE("2021-01-03")+B51+(A51-1)*7</f>
         <v>44260</v>
       </c>
-      <c r="D49" t="s">
-        <v>95</v>
-      </c>
-      <c r="E49">
+      <c r="D51" t="s">
+        <v>93</v>
+      </c>
+      <c r="E51">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>10</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1">
-        <f t="shared" si="1"/>
-        <v>44263</v>
-      </c>
-      <c r="D50" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>10</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" s="1">
-        <f t="shared" si="1"/>
-        <v>44263</v>
-      </c>
-      <c r="D51" t="s">
-        <v>96</v>
-      </c>
-      <c r="E51">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" t="s">
+        <v>214</v>
+      </c>
+      <c r="J51" t="s">
+        <v>203</v>
+      </c>
+      <c r="M51" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>10</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" si="1"/>
-        <v>44265</v>
+        <f>DATEVALUE("2021-01-03")+B52+(A52-1)*7</f>
+        <v>44263</v>
       </c>
       <c r="D52" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E52">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="F52" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" t="s">
+        <v>21</v>
+      </c>
+      <c r="J52" t="s">
+        <v>201</v>
+      </c>
+      <c r="M52" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>10</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" si="1"/>
-        <v>44265</v>
+        <f>DATEVALUE("2021-01-03")+B53+(A53-1)*7</f>
+        <v>44263</v>
       </c>
       <c r="D53" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>10</v>
       </c>
       <c r="B54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" si="1"/>
-        <v>44266</v>
+        <f>DATEVALUE("2021-01-03")+B54+(A54-1)*7</f>
+        <v>44265</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" t="s">
-        <v>11</v>
-      </c>
-      <c r="G54" t="s">
-        <v>52</v>
-      </c>
-      <c r="J54" t="s">
-        <v>71</v>
-      </c>
-      <c r="K54" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+      <c r="E54">
+        <v>25</v>
+      </c>
+      <c r="I54" t="s">
+        <v>216</v>
+      </c>
+      <c r="M54" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>10</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" si="1"/>
-        <v>44267</v>
+        <f>DATEVALUE("2021-01-03")+B55+(A55-1)*7</f>
+        <v>44265</v>
       </c>
       <c r="D55" t="s">
-        <v>98</v>
-      </c>
-      <c r="E55">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>10</v>
       </c>
       <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56" s="1">
+        <f>DATEVALUE("2021-01-03")+B56+(A56-1)*7</f>
+        <v>44266</v>
+      </c>
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" t="s">
+        <v>52</v>
+      </c>
+      <c r="J56" t="s">
+        <v>71</v>
+      </c>
+      <c r="K56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57">
         <v>5</v>
       </c>
-      <c r="C56" s="1">
-        <f t="shared" si="1"/>
+      <c r="C57" s="1">
+        <f>DATEVALUE("2021-01-03")+B57+(A57-1)*7</f>
         <v>44267</v>
       </c>
-      <c r="D56" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>11</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57" s="1">
-        <f t="shared" si="1"/>
-        <v>44270</v>
-      </c>
       <c r="D57" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+      <c r="E57">
+        <v>26</v>
+      </c>
+      <c r="I57" t="s">
+        <v>217</v>
+      </c>
+      <c r="M57" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C58" s="1">
-        <f t="shared" si="1"/>
-        <v>44270</v>
+        <f>DATEVALUE("2021-01-03")+B58+(A58-1)*7</f>
+        <v>44267</v>
       </c>
       <c r="D58" t="s">
         <v>99</v>
       </c>
-      <c r="E58">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>11</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" si="1"/>
-        <v>44271</v>
+        <f>DATEVALUE("2021-01-03")+B59+(A59-1)*7</f>
+        <v>44270</v>
       </c>
       <c r="D59" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="E59">
+        <v>27</v>
+      </c>
+      <c r="F59" t="s">
+        <v>8</v>
+      </c>
+      <c r="I59" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59" t="s">
+        <v>202</v>
+      </c>
+      <c r="M59" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>11</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C60" s="1">
-        <f t="shared" si="1"/>
-        <v>44272</v>
+        <f>DATEVALUE("2021-01-03")+B60+(A60-1)*7</f>
+        <v>44270</v>
       </c>
       <c r="D60" t="s">
-        <v>100</v>
-      </c>
-      <c r="E60">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>11</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C61" s="1">
-        <f t="shared" si="1"/>
-        <v>44273</v>
+        <f>DATEVALUE("2021-01-03")+B61+(A61-1)*7</f>
+        <v>44271</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
-      </c>
-      <c r="F61" t="s">
-        <v>11</v>
-      </c>
-      <c r="G61" t="s">
-        <v>52</v>
-      </c>
-      <c r="J61" t="s">
-        <v>72</v>
-      </c>
-      <c r="K61" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>11</v>
       </c>
       <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62" s="1">
+        <f>DATEVALUE("2021-01-03")+B62+(A62-1)*7</f>
+        <v>44272</v>
+      </c>
+      <c r="D62" t="s">
+        <v>198</v>
+      </c>
+      <c r="E62">
+        <v>28</v>
+      </c>
+      <c r="I62" t="s">
+        <v>220</v>
+      </c>
+      <c r="M62" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>11</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63" s="1">
+        <f>DATEVALUE("2021-01-03")+B63+(A63-1)*7</f>
+        <v>44273</v>
+      </c>
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" t="s">
+        <v>52</v>
+      </c>
+      <c r="J63" t="s">
+        <v>72</v>
+      </c>
+      <c r="K63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>11</v>
+      </c>
+      <c r="B64">
         <v>5</v>
       </c>
-      <c r="C62" s="1">
-        <f t="shared" si="1"/>
+      <c r="C64" s="1">
+        <f>DATEVALUE("2021-01-03")+B64+(A64-1)*7</f>
         <v>44274</v>
       </c>
-      <c r="D62" t="s">
-        <v>101</v>
-      </c>
-      <c r="E62">
+      <c r="D64" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64">
         <v>29</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>12</v>
-      </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63" s="1">
-        <f t="shared" si="1"/>
-        <v>44277</v>
-      </c>
-      <c r="D63" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>12</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64" s="1">
-        <f t="shared" si="1"/>
-        <v>44277</v>
-      </c>
-      <c r="D64" t="s">
-        <v>102</v>
-      </c>
-      <c r="E64">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I64" t="s">
+        <v>221</v>
+      </c>
+      <c r="M64" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>12</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C65" s="1">
-        <f t="shared" si="1"/>
-        <v>44279</v>
+        <f>DATEVALUE("2021-01-03")+B65+(A65-1)*7</f>
+        <v>44277</v>
       </c>
       <c r="D65" t="s">
-        <v>103</v>
+        <v>197</v>
       </c>
       <c r="E65">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="F65" t="s">
+        <v>8</v>
+      </c>
+      <c r="I65" t="s">
+        <v>225</v>
+      </c>
+      <c r="J65" t="s">
+        <v>204</v>
+      </c>
+      <c r="M65" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>12</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C66" s="1">
-        <f t="shared" ref="C66:C77" si="2">DATEVALUE("2021-01-03")+B66+(A66-1)*7</f>
-        <v>44279</v>
+        <f>DATEVALUE("2021-01-03")+B66+(A66-1)*7</f>
+        <v>44277</v>
       </c>
       <c r="D66" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>12</v>
       </c>
       <c r="B67">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C67" s="1">
-        <f t="shared" si="2"/>
-        <v>44280</v>
+        <f>DATEVALUE("2021-01-03")+B67+(A67-1)*7</f>
+        <v>44279</v>
       </c>
       <c r="D67" t="s">
-        <v>10</v>
+        <v>196</v>
+      </c>
+      <c r="E67">
+        <v>31</v>
       </c>
       <c r="F67" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" t="s">
-        <v>52</v>
+        <v>8</v>
+      </c>
+      <c r="I67" t="s">
+        <v>21</v>
       </c>
       <c r="J67" t="s">
-        <v>73</v>
-      </c>
-      <c r="K67" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+      <c r="M67" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>12</v>
       </c>
       <c r="B68">
+        <v>3</v>
+      </c>
+      <c r="C68" s="1">
+        <f>DATEVALUE("2021-01-03")+B68+(A68-1)*7</f>
+        <v>44279</v>
+      </c>
+      <c r="D68" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>12</v>
+      </c>
+      <c r="B69">
+        <v>4</v>
+      </c>
+      <c r="C69" s="1">
+        <f>DATEVALUE("2021-01-03")+B69+(A69-1)*7</f>
+        <v>44280</v>
+      </c>
+      <c r="D69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" t="s">
+        <v>52</v>
+      </c>
+      <c r="J69" t="s">
+        <v>73</v>
+      </c>
+      <c r="K69" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>12</v>
+      </c>
+      <c r="B70">
         <v>5</v>
       </c>
-      <c r="C68" s="1">
-        <f t="shared" si="2"/>
+      <c r="C70" s="1">
+        <f>DATEVALUE("2021-01-03")+B70+(A70-1)*7</f>
         <v>44281</v>
       </c>
-      <c r="D68" t="s">
-        <v>104</v>
-      </c>
-      <c r="E68">
+      <c r="D70" t="s">
+        <v>97</v>
+      </c>
+      <c r="E70">
         <v>32</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>13</v>
-      </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" s="1">
-        <f t="shared" si="2"/>
-        <v>44284</v>
-      </c>
-      <c r="D69" t="s">
-        <v>105</v>
-      </c>
-      <c r="E69">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>13</v>
-      </c>
-      <c r="B70">
-        <v>2</v>
-      </c>
-      <c r="C70" s="1">
-        <f t="shared" si="2"/>
-        <v>44285</v>
-      </c>
-      <c r="D70" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>8</v>
+      </c>
+      <c r="I70" t="s">
+        <v>226</v>
+      </c>
+      <c r="J70" t="s">
+        <v>208</v>
+      </c>
+      <c r="M70" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>13</v>
       </c>
       <c r="B71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C71" s="1">
-        <f t="shared" si="2"/>
-        <v>44286</v>
+        <f>DATEVALUE("2021-01-03")+B71+(A71-1)*7</f>
+        <v>44284</v>
       </c>
       <c r="D71" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E71">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="F71" t="s">
+        <v>8</v>
+      </c>
+      <c r="J71" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>13</v>
       </c>
       <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72" s="1">
+        <f>DATEVALUE("2021-01-03")+B72+(A72-1)*7</f>
+        <v>44285</v>
+      </c>
+      <c r="D72" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>13</v>
+      </c>
+      <c r="B73">
+        <v>3</v>
+      </c>
+      <c r="C73" s="1">
+        <f>DATEVALUE("2021-01-03")+B73+(A73-1)*7</f>
+        <v>44286</v>
+      </c>
+      <c r="D73" t="s">
+        <v>207</v>
+      </c>
+      <c r="E73">
+        <v>34</v>
+      </c>
+      <c r="H73" t="s">
+        <v>19</v>
+      </c>
+      <c r="L73" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>13</v>
+      </c>
+      <c r="B74">
         <v>4</v>
       </c>
-      <c r="C72" s="1">
-        <f t="shared" si="2"/>
+      <c r="C74" s="1">
+        <f>DATEVALUE("2021-01-03")+B74+(A74-1)*7</f>
         <v>44287</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D74" t="s">
         <v>51</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F74" t="s">
         <v>11</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G74" t="s">
         <v>52</v>
       </c>
-      <c r="J72" t="s">
+      <c r="J74" t="s">
         <v>48</v>
       </c>
-      <c r="K72" t="s">
+      <c r="K74" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>14</v>
-      </c>
-      <c r="B73">
-        <v>2</v>
-      </c>
-      <c r="C73" s="1">
-        <f t="shared" si="2"/>
-        <v>44292</v>
-      </c>
-      <c r="D73" t="s">
-        <v>53</v>
-      </c>
-      <c r="F73" t="s">
-        <v>11</v>
-      </c>
-      <c r="G73" t="s">
-        <v>52</v>
-      </c>
-      <c r="J73" t="s">
-        <v>49</v>
-      </c>
-      <c r="K73" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>14</v>
-      </c>
-      <c r="B74">
-        <v>3</v>
-      </c>
-      <c r="C74" s="1">
-        <f t="shared" si="2"/>
-        <v>44293</v>
-      </c>
-      <c r="D74" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>14</v>
       </c>
       <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75" s="1">
+        <f>DATEVALUE("2021-01-03")+B75+(A75-1)*7</f>
+        <v>44292</v>
+      </c>
+      <c r="D75" t="s">
+        <v>53</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" t="s">
+        <v>52</v>
+      </c>
+      <c r="J75" t="s">
+        <v>49</v>
+      </c>
+      <c r="K75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>14</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76" s="1">
+        <f>DATEVALUE("2021-01-03")+B76+(A76-1)*7</f>
+        <v>44293</v>
+      </c>
+      <c r="D76" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>14</v>
+      </c>
+      <c r="B77">
         <v>5</v>
       </c>
-      <c r="C75" s="1">
-        <f t="shared" si="2"/>
+      <c r="C77" s="1">
+        <f>DATEVALUE("2021-01-03")+B77+(A77-1)*7</f>
         <v>44295</v>
       </c>
-      <c r="D75" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>8</v>
-      </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-      <c r="C76" s="1">
-        <f t="shared" si="2"/>
-        <v>44249</v>
-      </c>
-      <c r="D76" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>9</v>
-      </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-      <c r="C77" s="1">
-        <f t="shared" si="2"/>
-        <v>44256</v>
-      </c>
       <c r="D77" t="s">
-        <v>173</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M75">
-    <sortCondition ref="C2:C75"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:M77">
+    <sortCondition ref="A31:A77"/>
+    <sortCondition ref="B31:B77"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update a week of lessons
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FB3A2A-F78D-BC4C-B16C-6250D2099908}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB30076E-BD26-294B-9A65-9B96F03F9CB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-71820" yWindow="2460" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="237">
   <si>
     <t>Date</t>
   </si>
@@ -724,6 +724,27 @@
   </si>
   <si>
     <t>#task-b11</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=78996e65-ca31-466c-bbf6-acd40181af1f</t>
+  </si>
+  <si>
+    <t>#data-sources</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=9c2e26ca-968f-4ecd-89e0-acd40185864f</t>
+  </si>
+  <si>
+    <t>#reproduce</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=beabb68d-78e2-49e4-9136-acd40189ef0c</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=ed2c66f6-9a8d-46ef-96f2-acd50003c117</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=15200ac3-1dbc-486d-b3b4-acd50008bc14</t>
   </si>
 </sst>
 </file>
@@ -1082,10 +1103,10 @@
   <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E18" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1146,7 +1167,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C33" si="0">DATEVALUE("2021-01-03")+B2+(A2-1)*7</f>
+        <f t="shared" ref="C2:C30" si="0">DATEVALUE("2021-01-03")+B2+(A2-1)*7</f>
         <v>44202</v>
       </c>
       <c r="D2" t="s">
@@ -2088,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="1">
-        <f>DATEVALUE("2021-01-03")+B31+(A31-1)*7</f>
+        <f t="shared" ref="C31:C77" si="1">DATEVALUE("2021-01-03")+B31+(A31-1)*7</f>
         <v>44235</v>
       </c>
       <c r="D31" t="s">
@@ -2103,7 +2124,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="1">
-        <f>DATEVALUE("2021-01-03")+B32+(A32-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44235</v>
       </c>
       <c r="D32" t="s">
@@ -2145,7 +2166,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="1">
-        <f>DATEVALUE("2021-01-03")+B33+(A33-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44236</v>
       </c>
       <c r="D33" t="s">
@@ -2166,7 +2187,7 @@
         <v>3</v>
       </c>
       <c r="C34" s="1">
-        <f>DATEVALUE("2021-01-03")+B34+(A34-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44237</v>
       </c>
       <c r="D34" t="s">
@@ -2181,7 +2202,7 @@
         <v>3</v>
       </c>
       <c r="C35" s="1">
-        <f>DATEVALUE("2021-01-03")+B35+(A35-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44237</v>
       </c>
       <c r="D35" t="s">
@@ -2223,7 +2244,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="1">
-        <f>DATEVALUE("2021-01-03")+B36+(A36-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44238</v>
       </c>
       <c r="D36" t="s">
@@ -2250,7 +2271,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="1">
-        <f>DATEVALUE("2021-01-03")+B37+(A37-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44239</v>
       </c>
       <c r="D37" t="s">
@@ -2292,7 +2313,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="1">
-        <f>DATEVALUE("2021-01-03")+B38+(A38-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44249</v>
       </c>
       <c r="D38" t="s">
@@ -2334,7 +2355,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="1">
-        <f>DATEVALUE("2021-01-03")+B39+(A39-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44249</v>
       </c>
       <c r="D39" t="s">
@@ -2349,7 +2370,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="1">
-        <f>DATEVALUE("2021-01-03")+B40+(A40-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44251</v>
       </c>
       <c r="D40" t="s">
@@ -2364,7 +2385,7 @@
         <v>3</v>
       </c>
       <c r="C41" s="1">
-        <f>DATEVALUE("2021-01-03")+B41+(A41-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44251</v>
       </c>
       <c r="D41" t="s">
@@ -2376,9 +2397,18 @@
       <c r="F41" t="s">
         <v>8</v>
       </c>
+      <c r="G41" t="s">
+        <v>3</v>
+      </c>
       <c r="I41" t="s">
         <v>21</v>
       </c>
+      <c r="J41" t="s">
+        <v>231</v>
+      </c>
+      <c r="K41" t="s">
+        <v>230</v>
+      </c>
       <c r="M41" t="s">
         <v>188</v>
       </c>
@@ -2391,7 +2421,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="1">
-        <f>DATEVALUE("2021-01-03")+B42+(A42-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44251</v>
       </c>
       <c r="D42" t="s">
@@ -2406,7 +2436,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="1">
-        <f>DATEVALUE("2021-01-03")+B43+(A43-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44252</v>
       </c>
       <c r="D43" t="s">
@@ -2433,7 +2463,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="1">
-        <f>DATEVALUE("2021-01-03")+B44+(A44-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44253</v>
       </c>
       <c r="D44" t="s">
@@ -2445,8 +2475,17 @@
       <c r="F44" t="s">
         <v>8</v>
       </c>
+      <c r="G44" t="s">
+        <v>3</v>
+      </c>
       <c r="I44" t="s">
         <v>190</v>
+      </c>
+      <c r="J44" t="s">
+        <v>233</v>
+      </c>
+      <c r="K44" t="s">
+        <v>232</v>
       </c>
       <c r="M44" t="s">
         <v>189</v>
@@ -2460,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="1">
-        <f>DATEVALUE("2021-01-03")+B45+(A45-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44256</v>
       </c>
       <c r="D45" t="s">
@@ -2472,6 +2511,9 @@
       <c r="F45" t="s">
         <v>8</v>
       </c>
+      <c r="G45" t="s">
+        <v>3</v>
+      </c>
       <c r="H45" t="s">
         <v>19</v>
       </c>
@@ -2480,6 +2522,9 @@
       </c>
       <c r="J45" t="s">
         <v>192</v>
+      </c>
+      <c r="K45" t="s">
+        <v>234</v>
       </c>
       <c r="L45" t="s">
         <v>187</v>
@@ -2496,7 +2541,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="1">
-        <f>DATEVALUE("2021-01-03")+B46+(A46-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44256</v>
       </c>
       <c r="D46" t="s">
@@ -2511,7 +2556,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="1">
-        <f>DATEVALUE("2021-01-03")+B47+(A47-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44256</v>
       </c>
       <c r="D47" t="s">
@@ -2526,7 +2571,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="1">
-        <f>DATEVALUE("2021-01-03")+B48+(A48-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44257</v>
       </c>
       <c r="D48" t="s">
@@ -2541,7 +2586,7 @@
         <v>3</v>
       </c>
       <c r="C49" s="1">
-        <f>DATEVALUE("2021-01-03")+B49+(A49-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44258</v>
       </c>
       <c r="D49" t="s">
@@ -2553,8 +2598,14 @@
       <c r="F49" t="s">
         <v>8</v>
       </c>
+      <c r="G49" t="s">
+        <v>3</v>
+      </c>
       <c r="J49" t="s">
         <v>191</v>
+      </c>
+      <c r="K49" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -2565,7 +2616,7 @@
         <v>4</v>
       </c>
       <c r="C50" s="1">
-        <f>DATEVALUE("2021-01-03")+B50+(A50-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44259</v>
       </c>
       <c r="D50" t="s">
@@ -2592,7 +2643,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="1">
-        <f>DATEVALUE("2021-01-03")+B51+(A51-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44260</v>
       </c>
       <c r="D51" t="s">
@@ -2604,11 +2655,17 @@
       <c r="F51" t="s">
         <v>8</v>
       </c>
+      <c r="G51" t="s">
+        <v>3</v>
+      </c>
       <c r="I51" t="s">
         <v>214</v>
       </c>
       <c r="J51" t="s">
         <v>203</v>
+      </c>
+      <c r="K51" t="s">
+        <v>236</v>
       </c>
       <c r="M51" t="s">
         <v>213</v>
@@ -2622,7 +2679,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="1">
-        <f>DATEVALUE("2021-01-03")+B52+(A52-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44263</v>
       </c>
       <c r="D52" t="s">
@@ -2652,7 +2709,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="1">
-        <f>DATEVALUE("2021-01-03")+B53+(A53-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44263</v>
       </c>
       <c r="D53" t="s">
@@ -2667,7 +2724,7 @@
         <v>3</v>
       </c>
       <c r="C54" s="1">
-        <f>DATEVALUE("2021-01-03")+B54+(A54-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44265</v>
       </c>
       <c r="D54" t="s">
@@ -2691,7 +2748,7 @@
         <v>3</v>
       </c>
       <c r="C55" s="1">
-        <f>DATEVALUE("2021-01-03")+B55+(A55-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44265</v>
       </c>
       <c r="D55" t="s">
@@ -2706,7 +2763,7 @@
         <v>4</v>
       </c>
       <c r="C56" s="1">
-        <f>DATEVALUE("2021-01-03")+B56+(A56-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44266</v>
       </c>
       <c r="D56" t="s">
@@ -2733,7 +2790,7 @@
         <v>5</v>
       </c>
       <c r="C57" s="1">
-        <f>DATEVALUE("2021-01-03")+B57+(A57-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44267</v>
       </c>
       <c r="D57" t="s">
@@ -2757,7 +2814,7 @@
         <v>5</v>
       </c>
       <c r="C58" s="1">
-        <f>DATEVALUE("2021-01-03")+B58+(A58-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44267</v>
       </c>
       <c r="D58" t="s">
@@ -2772,7 +2829,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="1">
-        <f>DATEVALUE("2021-01-03")+B59+(A59-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44270</v>
       </c>
       <c r="D59" t="s">
@@ -2802,7 +2859,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="1">
-        <f>DATEVALUE("2021-01-03")+B60+(A60-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44270</v>
       </c>
       <c r="D60" t="s">
@@ -2817,7 +2874,7 @@
         <v>2</v>
       </c>
       <c r="C61" s="1">
-        <f>DATEVALUE("2021-01-03")+B61+(A61-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44271</v>
       </c>
       <c r="D61" t="s">
@@ -2832,7 +2889,7 @@
         <v>3</v>
       </c>
       <c r="C62" s="1">
-        <f>DATEVALUE("2021-01-03")+B62+(A62-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44272</v>
       </c>
       <c r="D62" t="s">
@@ -2856,7 +2913,7 @@
         <v>4</v>
       </c>
       <c r="C63" s="1">
-        <f>DATEVALUE("2021-01-03")+B63+(A63-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44273</v>
       </c>
       <c r="D63" t="s">
@@ -2883,7 +2940,7 @@
         <v>5</v>
       </c>
       <c r="C64" s="1">
-        <f>DATEVALUE("2021-01-03")+B64+(A64-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44274</v>
       </c>
       <c r="D64" t="s">
@@ -2907,7 +2964,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="1">
-        <f>DATEVALUE("2021-01-03")+B65+(A65-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44277</v>
       </c>
       <c r="D65" t="s">
@@ -2937,7 +2994,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="1">
-        <f>DATEVALUE("2021-01-03")+B66+(A66-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44277</v>
       </c>
       <c r="D66" t="s">
@@ -2952,7 +3009,7 @@
         <v>3</v>
       </c>
       <c r="C67" s="1">
-        <f>DATEVALUE("2021-01-03")+B67+(A67-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44279</v>
       </c>
       <c r="D67" t="s">
@@ -2982,7 +3039,7 @@
         <v>3</v>
       </c>
       <c r="C68" s="1">
-        <f>DATEVALUE("2021-01-03")+B68+(A68-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44279</v>
       </c>
       <c r="D68" t="s">
@@ -2997,7 +3054,7 @@
         <v>4</v>
       </c>
       <c r="C69" s="1">
-        <f>DATEVALUE("2021-01-03")+B69+(A69-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44280</v>
       </c>
       <c r="D69" t="s">
@@ -3024,7 +3081,7 @@
         <v>5</v>
       </c>
       <c r="C70" s="1">
-        <f>DATEVALUE("2021-01-03")+B70+(A70-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44281</v>
       </c>
       <c r="D70" t="s">
@@ -3054,7 +3111,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="1">
-        <f>DATEVALUE("2021-01-03")+B71+(A71-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44284</v>
       </c>
       <c r="D71" t="s">
@@ -3078,7 +3135,7 @@
         <v>2</v>
       </c>
       <c r="C72" s="1">
-        <f>DATEVALUE("2021-01-03")+B72+(A72-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44285</v>
       </c>
       <c r="D72" t="s">
@@ -3093,7 +3150,7 @@
         <v>3</v>
       </c>
       <c r="C73" s="1">
-        <f>DATEVALUE("2021-01-03")+B73+(A73-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44286</v>
       </c>
       <c r="D73" t="s">
@@ -3117,7 +3174,7 @@
         <v>4</v>
       </c>
       <c r="C74" s="1">
-        <f>DATEVALUE("2021-01-03")+B74+(A74-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44287</v>
       </c>
       <c r="D74" t="s">
@@ -3144,7 +3201,7 @@
         <v>2</v>
       </c>
       <c r="C75" s="1">
-        <f>DATEVALUE("2021-01-03")+B75+(A75-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44292</v>
       </c>
       <c r="D75" t="s">
@@ -3171,7 +3228,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="1">
-        <f>DATEVALUE("2021-01-03")+B76+(A76-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44293</v>
       </c>
       <c r="D76" t="s">
@@ -3186,7 +3243,7 @@
         <v>5</v>
       </c>
       <c r="C77" s="1">
-        <f>DATEVALUE("2021-01-03")+B77+(A77-1)*7</f>
+        <f t="shared" si="1"/>
         <v>44295</v>
       </c>
       <c r="D77" t="s">

</xml_diff>

<commit_message>
Added missing image files
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB30076E-BD26-294B-9A65-9B96F03F9CB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80131A02-C4D1-A746-BAED-1C0A7FEB6F46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-71820" yWindow="2460" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -612,9 +612,6 @@
     <t>#mds</t>
   </si>
   <si>
-    <t>#PCA</t>
-  </si>
-  <si>
     <t>Task 11 due at 9 am</t>
   </si>
   <si>
@@ -745,6 +742,9 @@
   </si>
   <si>
     <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=15200ac3-1dbc-486d-b3b4-acd50008bc14</t>
+  </si>
+  <si>
+    <t>#pca</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1106,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E18" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K51" sqref="K51"/>
+      <selection pane="bottomRight" activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2389,7 +2389,7 @@
         <v>44251</v>
       </c>
       <c r="D41" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E41">
         <v>19</v>
@@ -2404,10 +2404,10 @@
         <v>21</v>
       </c>
       <c r="J41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M41" t="s">
         <v>188</v>
@@ -2482,10 +2482,10 @@
         <v>190</v>
       </c>
       <c r="J44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M44" t="s">
         <v>189</v>
@@ -2518,19 +2518,19 @@
         <v>19</v>
       </c>
       <c r="I45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J45" t="s">
-        <v>192</v>
+        <v>236</v>
       </c>
       <c r="K45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L45" t="s">
         <v>187</v>
       </c>
       <c r="M45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -2545,7 +2545,7 @@
         <v>44256</v>
       </c>
       <c r="D46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -2605,7 +2605,7 @@
         <v>191</v>
       </c>
       <c r="K49" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -2659,16 +2659,16 @@
         <v>3</v>
       </c>
       <c r="I51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J51" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M51" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -2695,10 +2695,10 @@
         <v>21</v>
       </c>
       <c r="J52" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
@@ -2713,7 +2713,7 @@
         <v>44263</v>
       </c>
       <c r="D53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -2728,16 +2728,16 @@
         <v>44265</v>
       </c>
       <c r="D54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E54">
         <v>25</v>
       </c>
       <c r="I54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -2794,16 +2794,16 @@
         <v>44267</v>
       </c>
       <c r="D57" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E57">
         <v>26</v>
       </c>
       <c r="I57" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -2845,10 +2845,10 @@
         <v>21</v>
       </c>
       <c r="J59" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M59" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
@@ -2893,16 +2893,16 @@
         <v>44272</v>
       </c>
       <c r="D62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E62">
         <v>28</v>
       </c>
       <c r="I62" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M62" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -2944,16 +2944,16 @@
         <v>44274</v>
       </c>
       <c r="D64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E64">
         <v>29</v>
       </c>
       <c r="I64" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M64" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
@@ -2968,7 +2968,7 @@
         <v>44277</v>
       </c>
       <c r="D65" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E65">
         <v>30</v>
@@ -2977,13 +2977,13 @@
         <v>8</v>
       </c>
       <c r="I65" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J65" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M65" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
@@ -3013,7 +3013,7 @@
         <v>44279</v>
       </c>
       <c r="D67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E67">
         <v>31</v>
@@ -3025,10 +3025,10 @@
         <v>21</v>
       </c>
       <c r="J67" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M67" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
@@ -3094,13 +3094,13 @@
         <v>8</v>
       </c>
       <c r="I70" t="s">
+        <v>225</v>
+      </c>
+      <c r="J70" t="s">
+        <v>207</v>
+      </c>
+      <c r="M70" t="s">
         <v>226</v>
-      </c>
-      <c r="J70" t="s">
-        <v>208</v>
-      </c>
-      <c r="M70" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
@@ -3124,7 +3124,7 @@
         <v>8</v>
       </c>
       <c r="J71" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
@@ -3154,7 +3154,7 @@
         <v>44286</v>
       </c>
       <c r="D73" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E73">
         <v>34</v>
@@ -3163,7 +3163,7 @@
         <v>19</v>
       </c>
       <c r="L73" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated schedule, fixed slide errors
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8603942E-EDCF-504C-BDDE-7237741DCFB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFB7D12-1244-064E-B7C5-2EDA98D1C4D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-71820" yWindow="2460" windowWidth="28040" windowHeight="17040" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
+    <workbookView xWindow="-30680" yWindow="-2640" windowWidth="28800" windowHeight="17540" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="248">
   <si>
     <t>Date</t>
   </si>
@@ -633,9 +633,6 @@
     <t>Alternatives to maps</t>
   </si>
   <si>
-    <t>Cleaning and validating data</t>
-  </si>
-  <si>
     <t>#slides</t>
   </si>
   <si>
@@ -751,6 +748,36 @@
   </si>
   <si>
     <t>#mapping-2</t>
+  </si>
+  <si>
+    <t>slides/20-MDS.html</t>
+  </si>
+  <si>
+    <t>slides/21-k-means.html</t>
+  </si>
+  <si>
+    <t>Rpres</t>
+  </si>
+  <si>
+    <t>slides/20-slide-presentation.Rpres</t>
+  </si>
+  <si>
+    <t>slides/20-slide-presentation.html</t>
+  </si>
+  <si>
+    <t>slides/25-testing.html</t>
+  </si>
+  <si>
+    <t>#testing</t>
+  </si>
+  <si>
+    <t>Checking your work</t>
+  </si>
+  <si>
+    <t>slides/18a-finding-data.html</t>
+  </si>
+  <si>
+    <t>slides/18b-reproducible-reports.html</t>
   </si>
 </sst>
 </file>
@@ -1109,10 +1136,10 @@
   <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E27" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E33" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J63" sqref="J63"/>
+      <selection pane="bottomRight" activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2406,14 +2433,20 @@
       <c r="G41" t="s">
         <v>3</v>
       </c>
+      <c r="H41" t="s">
+        <v>19</v>
+      </c>
       <c r="I41" t="s">
         <v>21</v>
       </c>
       <c r="J41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K41" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="L41" t="s">
+        <v>246</v>
       </c>
       <c r="M41" t="s">
         <v>188</v>
@@ -2484,14 +2517,20 @@
       <c r="G44" t="s">
         <v>3</v>
       </c>
+      <c r="H44" t="s">
+        <v>19</v>
+      </c>
       <c r="I44" t="s">
         <v>190</v>
       </c>
       <c r="J44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K44" t="s">
-        <v>231</v>
+        <v>230</v>
+      </c>
+      <c r="L44" t="s">
+        <v>247</v>
       </c>
       <c r="M44" t="s">
         <v>189</v>
@@ -2524,19 +2563,19 @@
         <v>19</v>
       </c>
       <c r="I45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J45" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L45" t="s">
         <v>187</v>
       </c>
       <c r="M45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -2607,11 +2646,17 @@
       <c r="G49" t="s">
         <v>3</v>
       </c>
+      <c r="H49" t="s">
+        <v>19</v>
+      </c>
       <c r="J49" t="s">
         <v>191</v>
       </c>
       <c r="K49" t="s">
-        <v>234</v>
+        <v>233</v>
+      </c>
+      <c r="L49" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -2664,17 +2709,23 @@
       <c r="G51" t="s">
         <v>3</v>
       </c>
+      <c r="H51" t="s">
+        <v>19</v>
+      </c>
       <c r="I51" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J51" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K51" t="s">
-        <v>235</v>
+        <v>234</v>
+      </c>
+      <c r="L51" t="s">
+        <v>239</v>
       </c>
       <c r="M51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -2697,14 +2748,26 @@
       <c r="F52" t="s">
         <v>8</v>
       </c>
+      <c r="G52" t="s">
+        <v>240</v>
+      </c>
+      <c r="H52" t="s">
+        <v>19</v>
+      </c>
       <c r="I52" t="s">
         <v>21</v>
       </c>
       <c r="J52" t="s">
-        <v>200</v>
+        <v>199</v>
+      </c>
+      <c r="K52" t="s">
+        <v>241</v>
+      </c>
+      <c r="L52" t="s">
+        <v>242</v>
       </c>
       <c r="M52" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
@@ -2734,16 +2797,28 @@
         <v>44265</v>
       </c>
       <c r="D54" t="s">
-        <v>199</v>
+        <v>245</v>
       </c>
       <c r="E54">
         <v>25</v>
       </c>
+      <c r="F54" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" t="s">
+        <v>19</v>
+      </c>
       <c r="I54" t="s">
-        <v>215</v>
+        <v>214</v>
+      </c>
+      <c r="J54" t="s">
+        <v>244</v>
+      </c>
+      <c r="L54" t="s">
+        <v>243</v>
       </c>
       <c r="M54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -2800,16 +2875,16 @@
         <v>44267</v>
       </c>
       <c r="D57" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E57">
         <v>26</v>
       </c>
       <c r="I57" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M57" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -2851,10 +2926,10 @@
         <v>21</v>
       </c>
       <c r="J59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M59" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
@@ -2908,13 +2983,13 @@
         <v>8</v>
       </c>
       <c r="I62" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J62" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M62" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -2965,13 +3040,13 @@
         <v>8</v>
       </c>
       <c r="I64" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
@@ -2995,13 +3070,13 @@
         <v>8</v>
       </c>
       <c r="I65" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J65" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M65" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
@@ -3043,10 +3118,10 @@
         <v>21</v>
       </c>
       <c r="J67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M67" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
@@ -3112,13 +3187,13 @@
         <v>8</v>
       </c>
       <c r="I70" t="s">
+        <v>224</v>
+      </c>
+      <c r="J70" t="s">
+        <v>206</v>
+      </c>
+      <c r="M70" t="s">
         <v>225</v>
-      </c>
-      <c r="J70" t="s">
-        <v>207</v>
-      </c>
-      <c r="M70" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
@@ -3142,7 +3217,7 @@
         <v>8</v>
       </c>
       <c r="J71" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
@@ -3172,7 +3247,7 @@
         <v>44286</v>
       </c>
       <c r="D73" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E73">
         <v>34</v>
@@ -3181,7 +3256,7 @@
         <v>19</v>
       </c>
       <c r="L73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated schedule, live coding 8
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Stats-data-visualization/01-course-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFB7D12-1244-064E-B7C5-2EDA98D1C4D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCE2035-36BB-6948-935C-6F7A4F397B7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30680" yWindow="-2640" windowWidth="28800" windowHeight="17540" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="250">
   <si>
     <t>Date</t>
   </si>
@@ -705,21 +705,12 @@
     <t>#task-18</t>
   </si>
   <si>
-    <t>Task 19</t>
-  </si>
-  <si>
-    <t>Task 20</t>
-  </si>
-  <si>
     <t>#task-20</t>
   </si>
   <si>
     <t>#task-19</t>
   </si>
   <si>
-    <t>#task-b11</t>
-  </si>
-  <si>
     <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=78996e65-ca31-466c-bbf6-acd40181af1f</t>
   </si>
   <si>
@@ -778,6 +769,21 @@
   </si>
   <si>
     <t>slides/18b-reproducible-reports.html</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=09743375-5dbd-435e-ae66-ace000173c94</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=d0565af8-95d9-495f-a782-ace0001aa7d3</t>
+  </si>
+  <si>
+    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=8f0f14d9-ddfc-47b5-87fb-ace0002155dd</t>
+  </si>
+  <si>
+    <t>#dynamic</t>
+  </si>
+  <si>
+    <t>slides/26-dynamic-graphics.html</t>
   </si>
 </sst>
 </file>
@@ -1136,10 +1142,10 @@
   <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E33" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E40" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L45" sqref="L45"/>
+      <selection pane="bottomRight" activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2440,13 +2446,13 @@
         <v>21</v>
       </c>
       <c r="J41" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K41" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="L41" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M41" t="s">
         <v>188</v>
@@ -2524,13 +2530,13 @@
         <v>190</v>
       </c>
       <c r="J44" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="K44" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="L44" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M44" t="s">
         <v>189</v>
@@ -2566,10 +2572,10 @@
         <v>209</v>
       </c>
       <c r="J45" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="K45" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L45" t="s">
         <v>187</v>
@@ -2653,10 +2659,10 @@
         <v>191</v>
       </c>
       <c r="K49" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="L49" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -2719,10 +2725,10 @@
         <v>201</v>
       </c>
       <c r="K51" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L51" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M51" t="s">
         <v>211</v>
@@ -2749,25 +2755,25 @@
         <v>8</v>
       </c>
       <c r="G52" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H52" t="s">
         <v>19</v>
       </c>
       <c r="I52" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="J52" t="s">
         <v>199</v>
       </c>
       <c r="K52" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="L52" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="M52" t="s">
-        <v>213</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
@@ -2797,7 +2803,7 @@
         <v>44265</v>
       </c>
       <c r="D54" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E54">
         <v>25</v>
@@ -2805,17 +2811,20 @@
       <c r="F54" t="s">
         <v>8</v>
       </c>
+      <c r="G54" t="s">
+        <v>3</v>
+      </c>
       <c r="H54" t="s">
         <v>19</v>
       </c>
-      <c r="I54" t="s">
-        <v>214</v>
-      </c>
       <c r="J54" t="s">
-        <v>244</v>
+        <v>241</v>
+      </c>
+      <c r="K54" t="s">
+        <v>246</v>
       </c>
       <c r="L54" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M54" t="s">
         <v>216</v>
@@ -2880,8 +2889,23 @@
       <c r="E57">
         <v>26</v>
       </c>
-      <c r="I57" t="s">
-        <v>215</v>
+      <c r="F57" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" t="s">
+        <v>3</v>
+      </c>
+      <c r="H57" t="s">
+        <v>19</v>
+      </c>
+      <c r="J57" t="s">
+        <v>248</v>
+      </c>
+      <c r="K57" t="s">
+        <v>247</v>
+      </c>
+      <c r="L57" t="s">
+        <v>249</v>
       </c>
       <c r="M57" t="s">
         <v>217</v>
@@ -2929,19 +2953,19 @@
         <v>200</v>
       </c>
       <c r="M59" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" s="1">
         <f t="shared" si="1"/>
-        <v>44270</v>
+        <v>44277</v>
       </c>
       <c r="D60" t="s">
         <v>120</v>
@@ -2983,10 +3007,10 @@
         <v>8</v>
       </c>
       <c r="I62" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J62" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="M62" t="s">
         <v>221</v>
@@ -3040,10 +3064,10 @@
         <v>8</v>
       </c>
       <c r="I64" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="J64" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M64" t="s">
         <v>222</v>
@@ -3070,25 +3094,25 @@
         <v>8</v>
       </c>
       <c r="I65" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="J65" t="s">
         <v>202</v>
       </c>
       <c r="M65" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" s="1">
         <f t="shared" si="1"/>
-        <v>44277</v>
+        <v>44284</v>
       </c>
       <c r="D66" t="s">
         <v>121</v>
@@ -3121,7 +3145,7 @@
         <v>203</v>
       </c>
       <c r="M67" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
@@ -3187,13 +3211,13 @@
         <v>8</v>
       </c>
       <c r="I70" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="J70" t="s">
         <v>206</v>
       </c>
       <c r="M70" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>